<commit_message>
update 17 december morning
</commit_message>
<xml_diff>
--- a/Dataset/raw/12 Desember 2024.xlsx
+++ b/Dataset/raw/12 Desember 2024.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Videos\POLYTRON\Job\Dataset\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8ECDCB3-B9F2-4C4E-AFCC-856019316A5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9229B3C6-B7C0-4404-A1B4-396FCDE6D235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="baking_12_december" sheetId="2" r:id="rId1"/>
     <sheet name="baking_13" sheetId="3" r:id="rId2"/>
+    <sheet name="baking_16" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1689" uniqueCount="394">
   <si>
     <t>No</t>
   </si>
@@ -749,14 +750,474 @@
   </si>
   <si>
     <t>14/12/24</t>
+  </si>
+  <si>
+    <t>MF49B0257</t>
+  </si>
+  <si>
+    <t>0HC1F5849B306K</t>
+  </si>
+  <si>
+    <t>16/12/24</t>
+  </si>
+  <si>
+    <t>0HC1F5849B306J</t>
+  </si>
+  <si>
+    <t>0HC1F5849B306H</t>
+  </si>
+  <si>
+    <t>0HC1F5849B306F</t>
+  </si>
+  <si>
+    <t>0HC1F5849B306E</t>
+  </si>
+  <si>
+    <t>0HC1F5849B306C</t>
+  </si>
+  <si>
+    <t>0HC1F5849B3066</t>
+  </si>
+  <si>
+    <t>0HC1F5849B3068</t>
+  </si>
+  <si>
+    <t>0HC1F5849B306A</t>
+  </si>
+  <si>
+    <t>0HC1F5849B3072</t>
+  </si>
+  <si>
+    <t>0HC1F5849B3070</t>
+  </si>
+  <si>
+    <t>0HC1F5849B306Z</t>
+  </si>
+  <si>
+    <t>0HC1F5849B306W</t>
+  </si>
+  <si>
+    <t>0HC1F5849B306V</t>
+  </si>
+  <si>
+    <t>0HC1F5849B306S</t>
+  </si>
+  <si>
+    <t>0HC1F5849B306Q</t>
+  </si>
+  <si>
+    <t>0HC1F5849B306N</t>
+  </si>
+  <si>
+    <t>0HC1F5849B306M</t>
+  </si>
+  <si>
+    <t>MF49C0095</t>
+  </si>
+  <si>
+    <t>0HC1F5849C303W</t>
+  </si>
+  <si>
+    <t>0HC1F5849C303T</t>
+  </si>
+  <si>
+    <t>0HC1F5849C303R</t>
+  </si>
+  <si>
+    <t>0HC1F5849C303P</t>
+  </si>
+  <si>
+    <t>0HC1F5849C303M</t>
+  </si>
+  <si>
+    <t>0HC1F5849C303J</t>
+  </si>
+  <si>
+    <t>0HC1F5849C303G</t>
+  </si>
+  <si>
+    <t>0HC1F5849C303E</t>
+  </si>
+  <si>
+    <t>0HC1F5849C303B</t>
+  </si>
+  <si>
+    <t>0HC1F5849C302Z</t>
+  </si>
+  <si>
+    <t>0HC1F5849C302Y</t>
+  </si>
+  <si>
+    <t>0HC1F5849C302W</t>
+  </si>
+  <si>
+    <t>0HC1F5849C302T</t>
+  </si>
+  <si>
+    <t>0HC1F5849C302R</t>
+  </si>
+  <si>
+    <t>0HC1F5849C302Q</t>
+  </si>
+  <si>
+    <t>0HC1F5849C302N</t>
+  </si>
+  <si>
+    <t>0HC1F5849C302L</t>
+  </si>
+  <si>
+    <t>0HC1F5849C302H</t>
+  </si>
+  <si>
+    <t>MF49C0127</t>
+  </si>
+  <si>
+    <t>0HC1F5849C304D</t>
+  </si>
+  <si>
+    <t>0HC1F5849C304C</t>
+  </si>
+  <si>
+    <t>0HC1F5849C304B</t>
+  </si>
+  <si>
+    <t>0HC1F5849C3049</t>
+  </si>
+  <si>
+    <t>0HC1F5849C3047</t>
+  </si>
+  <si>
+    <t>0HC1F5849C3045</t>
+  </si>
+  <si>
+    <t>0HC1F5849C3043</t>
+  </si>
+  <si>
+    <t>0HC1F5849C3041</t>
+  </si>
+  <si>
+    <t>0HC1F5849C303Z</t>
+  </si>
+  <si>
+    <t>0HC1F5849C304Y</t>
+  </si>
+  <si>
+    <t>0HC1F5849C304X</t>
+  </si>
+  <si>
+    <t>0HC1F5849C304T</t>
+  </si>
+  <si>
+    <t>0HC1F5849C304R</t>
+  </si>
+  <si>
+    <t>0HC1F5849C304Q</t>
+  </si>
+  <si>
+    <t>0HC1F5849C304N</t>
+  </si>
+  <si>
+    <t>0HC1F5849C304L</t>
+  </si>
+  <si>
+    <t>0HC1F5849C304J</t>
+  </si>
+  <si>
+    <t>0HC1F5849C304G</t>
+  </si>
+  <si>
+    <t>MF49C0190</t>
+  </si>
+  <si>
+    <t>0HC1F5849C307Y</t>
+  </si>
+  <si>
+    <t>0HC1F5849C307X</t>
+  </si>
+  <si>
+    <t>0HC1F5849C307W</t>
+  </si>
+  <si>
+    <t>0HC1F5849C307V</t>
+  </si>
+  <si>
+    <t>0HC1F5849C307T</t>
+  </si>
+  <si>
+    <t>0HC1F5849C307R</t>
+  </si>
+  <si>
+    <t>0HC1F5849C307Q</t>
+  </si>
+  <si>
+    <t>0HC1F5849C307P</t>
+  </si>
+  <si>
+    <t>0HC1F5849C307N</t>
+  </si>
+  <si>
+    <t>0HC1F5849C307E</t>
+  </si>
+  <si>
+    <t>0HC1F5849C3079</t>
+  </si>
+  <si>
+    <t>0HC1F5849C3075</t>
+  </si>
+  <si>
+    <t>0HC1F5849C306T</t>
+  </si>
+  <si>
+    <t>0HC1F5849C3070</t>
+  </si>
+  <si>
+    <t>0HC1F5849C306P</t>
+  </si>
+  <si>
+    <t>0HC1F5849C306R</t>
+  </si>
+  <si>
+    <t>0HC1F5849C306W</t>
+  </si>
+  <si>
+    <t>0HC1F5849C306Y</t>
+  </si>
+  <si>
+    <t>MF4990163</t>
+  </si>
+  <si>
+    <t>0KC1FKH499302B</t>
+  </si>
+  <si>
+    <t>0KC1FKH499302A</t>
+  </si>
+  <si>
+    <t>0KC1FKH4993029</t>
+  </si>
+  <si>
+    <t>0KC1FKH4993028</t>
+  </si>
+  <si>
+    <t>0KC1FKH4993027</t>
+  </si>
+  <si>
+    <t>0KC1FKH4993026</t>
+  </si>
+  <si>
+    <t>0KC1FKH4993025</t>
+  </si>
+  <si>
+    <t>0KC1FKH4993024</t>
+  </si>
+  <si>
+    <t>0KC1FKH4993022</t>
+  </si>
+  <si>
+    <t>0KC1FKH4993023</t>
+  </si>
+  <si>
+    <t>0KC1FKH4993021</t>
+  </si>
+  <si>
+    <t>0KC1FKH4993020</t>
+  </si>
+  <si>
+    <t>0KC1FKH499301Z</t>
+  </si>
+  <si>
+    <t>0KC1FKH499301Y</t>
+  </si>
+  <si>
+    <t>0KC1FKH499301X</t>
+  </si>
+  <si>
+    <t>0KC1FKH499301W</t>
+  </si>
+  <si>
+    <t>0KC1FKH499301R</t>
+  </si>
+  <si>
+    <t>0KC1FKH499301T</t>
+  </si>
+  <si>
+    <t>MF49A0201</t>
+  </si>
+  <si>
+    <t>0KC1FKH49A3026</t>
+  </si>
+  <si>
+    <t>0KC1FKH49A3025</t>
+  </si>
+  <si>
+    <t>0KC1FKH49A3024</t>
+  </si>
+  <si>
+    <t>0KC1FKH49A3023</t>
+  </si>
+  <si>
+    <t>0KC1FKH49A3022</t>
+  </si>
+  <si>
+    <t>0KC1FKH49A3021</t>
+  </si>
+  <si>
+    <t>0KC1FKH49A3020</t>
+  </si>
+  <si>
+    <t>0KC1FKH49A301Z</t>
+  </si>
+  <si>
+    <t>0KC1FKH49A301X</t>
+  </si>
+  <si>
+    <t>0KC1FKH49A301W</t>
+  </si>
+  <si>
+    <t>0KC1FKH49A301V</t>
+  </si>
+  <si>
+    <t>0KC1FKH49A301T</t>
+  </si>
+  <si>
+    <t>0KC1FKH49A301S</t>
+  </si>
+  <si>
+    <t>0KC1FKH49A301R</t>
+  </si>
+  <si>
+    <t>0KC1FKH49A301Q</t>
+  </si>
+  <si>
+    <t>0KC1FKH49A300J</t>
+  </si>
+  <si>
+    <t>0KC1FKH49A301N</t>
+  </si>
+  <si>
+    <t>0KC1FKH49A301P</t>
+  </si>
+  <si>
+    <t>MF49C0056</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C300X</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C300W</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C300V</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C300T</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C300S</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C300R</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C300Q</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C300P</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C300N</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C3016</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C3015</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C3014</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C3013</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C3012</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C3011</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C3010</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C300Z</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C300Y</t>
+  </si>
+  <si>
+    <t>MF49B0195</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B302C</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B302B</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B302A</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B3029</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B3028</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B3023</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B3027</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B3026</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B3025</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B302M</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B302L</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B302K</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B302J</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B302H</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B302G</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B302F</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B302E</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B302D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="166" formatCode="[$-13809]dd/mm/yy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -820,7 +1281,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -857,12 +1318,25 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="표준_~2585981" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3355,7 +3829,7 @@
     <mergeCell ref="D1:D2"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3366,8 +3840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+    <sheetView topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7614,11 +8088,4272 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="F3:F146 H3:H146" twoDigitTextYear="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A836090B-1D84-488F-9E82-01BA25B98056}">
+  <dimension ref="A1:I146"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="13"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="E3" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I3" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="E4" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I4" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="E5" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I5" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="E6" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I6" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="E7" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G7" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I7" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="E8" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G8" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I8" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="E9" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I9" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="E10" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I10" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="E11" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G11" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I11" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="7">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="E12" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I12" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="E13" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G13" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I13" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="E14" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G14" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I14" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="7">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="E15" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G15" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I15" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="7">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="E16" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G16" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I16" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="7">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="E17" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G17" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I17" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="7">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="E18" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G18" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I18" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="7">
+        <v>17</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="E19" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G19" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I19" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="7">
+        <v>18</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="E20" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G20" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I20" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="7">
+        <v>19</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="E21" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G21" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I21" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="7">
+        <v>20</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="E22" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G22" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I22" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="7">
+        <v>21</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="E23" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G23" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I23" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="7">
+        <v>22</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="E24" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G24" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I24" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="7">
+        <v>23</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="E25" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G25" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I25" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="7">
+        <v>24</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="E26" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G26" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I26" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="7">
+        <v>25</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="E27" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G27" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I27" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="7">
+        <v>26</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="E28" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G28" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I28" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="7">
+        <v>27</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="E29" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G29" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I29" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="7">
+        <v>28</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="E30" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G30" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I30" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="7">
+        <v>29</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="E31" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G31" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I31" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="7">
+        <v>30</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="E32" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G32" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I32" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="7">
+        <v>31</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="E33" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G33" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I33" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="7">
+        <v>32</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="E34" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G34" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I34" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="7">
+        <v>33</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="E35" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G35" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I35" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="7">
+        <v>34</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="E36" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G36" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I36" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="7">
+        <v>35</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="E37" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G37" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I37" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="7">
+        <v>36</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="E38" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G38" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I38" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="7">
+        <v>37</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="E39" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G39" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I39" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="7">
+        <v>38</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="E40" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G40" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I40" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="7">
+        <v>39</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="E41" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G41" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I41" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="7">
+        <v>40</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="E42" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G42" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I42" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="7">
+        <v>41</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="E43" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G43" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I43" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="7">
+        <v>42</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="E44" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G44" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I44" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="7">
+        <v>43</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="E45" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G45" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I45" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="7">
+        <v>44</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="E46" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G46" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I46" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="7">
+        <v>45</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="E47" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G47" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I47" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="7">
+        <v>46</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="E48" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G48" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I48" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="7">
+        <v>47</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="E49" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G49" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I49" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="7">
+        <v>48</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="E50" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G50" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I50" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="7">
+        <v>49</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="E51" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G51" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I51" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="7">
+        <v>50</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="E52" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G52" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I52" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="7">
+        <v>51</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="E53" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G53" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H53" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I53" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="7">
+        <v>52</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="E54" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G54" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I54" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="7">
+        <v>53</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="E55" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G55" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I55" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="7">
+        <v>54</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="E56" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G56" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I56" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="7">
+        <v>55</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="E57" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G57" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H57" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I57" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="7">
+        <v>56</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="E58" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G58" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H58" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I58" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="7">
+        <v>57</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="E59" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G59" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H59" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I59" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="7">
+        <v>58</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="E60" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G60" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H60" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I60" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="7">
+        <v>59</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="E61" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G61" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H61" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I61" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="7">
+        <v>60</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="E62" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G62" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H62" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I62" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="7">
+        <v>61</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>306</v>
+      </c>
+      <c r="E63" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G63" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I63" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="7">
+        <v>62</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="E64" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G64" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H64" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I64" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="7">
+        <v>63</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="E65" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G65" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H65" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I65" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="7">
+        <v>64</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="E66" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G66" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H66" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I66" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="7">
+        <v>65</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="E67" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G67" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H67" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I67" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="7">
+        <v>66</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="E68" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G68" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H68" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I68" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="7">
+        <v>67</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="D69" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="E69" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G69" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H69" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I69" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="7">
+        <v>68</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="D70" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="E70" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G70" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H70" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I70" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="7">
+        <v>69</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="D71" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="E71" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G71" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H71" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I71" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="7">
+        <v>70</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C72" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="D72" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="E72" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G72" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H72" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I72" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="7">
+        <v>71</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="D73" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="E73" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G73" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H73" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I73" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="7">
+        <v>72</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="D74" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="E74" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G74" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H74" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I74" s="10">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="7">
+        <v>73</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="E75" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G75" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H75" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I75" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="7">
+        <v>74</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="E76" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G76" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H76" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I76" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="7">
+        <v>75</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="E77" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G77" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H77" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I77" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="7">
+        <v>76</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="E78" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F78" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G78" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H78" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I78" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="7">
+        <v>77</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="E79" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F79" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G79" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H79" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I79" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="7">
+        <v>78</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="E80" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G80" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H80" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I80" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="7">
+        <v>79</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="E81" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G81" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H81" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I81" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="7">
+        <v>80</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="E82" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G82" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H82" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I82" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="7">
+        <v>81</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="E83" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G83" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H83" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I83" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="7">
+        <v>82</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="E84" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F84" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G84" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H84" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I84" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="7">
+        <v>83</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="E85" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F85" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G85" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H85" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I85" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="7">
+        <v>84</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="E86" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F86" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G86" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H86" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I86" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="7">
+        <v>85</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="E87" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F87" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G87" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H87" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I87" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="7">
+        <v>86</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="E88" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F88" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G88" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H88" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I88" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="7">
+        <v>87</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="E89" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F89" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G89" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H89" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I89" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="7">
+        <v>88</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="D90" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E90" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F90" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G90" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H90" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I90" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="7">
+        <v>89</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="E91" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F91" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G91" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H91" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I91" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="7">
+        <v>90</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="D92" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="E92" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F92" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G92" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H92" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I92" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="7">
+        <v>91</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="D93" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="E93" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F93" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G93" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H93" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I93" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="7">
+        <v>92</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="E94" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F94" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G94" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H94" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I94" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="7">
+        <v>93</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="E95" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F95" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G95" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H95" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I95" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="7">
+        <v>94</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="E96" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F96" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G96" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H96" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I96" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="7">
+        <v>95</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="E97" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F97" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G97" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H97" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I97" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="7">
+        <v>96</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C98" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="D98" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="E98" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F98" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G98" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H98" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I98" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="7">
+        <v>97</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="D99" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="E99" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F99" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G99" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H99" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I99" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="7">
+        <v>98</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C100" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="D100" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="E100" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F100" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G100" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H100" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I100" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="7">
+        <v>99</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C101" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="D101" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="E101" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F101" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G101" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H101" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I101" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="7">
+        <v>100</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C102" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="D102" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="E102" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F102" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G102" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H102" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I102" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="7">
+        <v>101</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C103" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="D103" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="E103" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F103" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G103" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H103" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I103" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="7">
+        <v>102</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C104" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="D104" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="E104" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F104" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G104" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H104" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I104" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="7">
+        <v>103</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C105" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="D105" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="E105" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F105" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G105" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H105" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I105" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="7">
+        <v>104</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C106" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="D106" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="E106" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F106" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G106" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H106" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I106" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="7">
+        <v>105</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C107" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="D107" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="E107" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F107" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G107" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H107" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I107" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="7">
+        <v>106</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C108" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="D108" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="E108" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F108" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G108" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H108" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I108" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="7">
+        <v>107</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C109" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="D109" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="E109" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F109" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G109" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H109" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I109" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="7">
+        <v>108</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C110" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="D110" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="E110" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F110" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G110" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H110" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I110" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="7">
+        <v>109</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C111" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="D111" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="E111" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F111" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G111" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H111" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I111" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="7">
+        <v>110</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C112" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="D112" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="E112" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F112" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G112" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H112" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I112" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="7">
+        <v>111</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C113" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="D113" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="E113" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F113" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G113" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H113" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I113" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="7">
+        <v>112</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C114" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="D114" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="E114" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F114" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G114" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H114" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I114" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="7">
+        <v>113</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C115" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="D115" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="E115" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F115" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G115" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H115" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I115" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="7">
+        <v>114</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C116" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="D116" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="E116" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F116" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G116" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H116" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I116" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="7">
+        <v>115</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C117" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="D117" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="E117" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F117" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G117" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H117" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I117" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="7">
+        <v>116</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C118" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="D118" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="E118" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F118" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G118" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H118" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I118" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="7">
+        <v>117</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C119" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="D119" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="E119" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F119" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G119" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H119" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I119" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="7">
+        <v>118</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C120" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="D120" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="E120" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F120" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G120" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H120" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I120" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="7">
+        <v>119</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C121" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="D121" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="E121" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F121" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G121" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H121" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I121" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="7">
+        <v>120</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C122" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="D122" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="E122" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F122" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G122" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H122" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I122" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="7">
+        <v>121</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C123" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="D123" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="E123" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F123" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G123" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H123" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I123" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="7">
+        <v>122</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C124" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="D124" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="E124" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F124" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G124" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H124" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I124" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="7">
+        <v>123</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C125" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="D125" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="E125" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F125" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G125" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H125" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I125" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A126" s="7">
+        <v>124</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C126" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="D126" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="E126" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F126" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G126" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H126" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I126" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="7">
+        <v>125</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C127" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="D127" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="E127" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F127" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G127" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H127" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I127" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="7">
+        <v>126</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C128" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="D128" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="E128" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F128" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G128" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H128" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I128" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="7">
+        <v>127</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C129" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="D129" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="E129" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F129" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G129" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H129" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I129" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="7">
+        <v>128</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C130" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="D130" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="E130" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F130" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G130" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H130" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I130" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="7">
+        <v>129</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C131" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="D131" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="E131" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F131" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G131" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H131" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I131" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="7">
+        <v>130</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C132" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="D132" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="E132" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F132" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G132" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H132" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I132" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="7">
+        <v>131</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C133" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="D133" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="E133" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F133" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G133" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H133" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I133" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A134" s="7">
+        <v>132</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C134" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="D134" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="E134" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F134" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G134" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H134" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I134" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A135" s="7">
+        <v>133</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C135" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="D135" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="E135" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F135" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G135" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H135" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I135" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A136" s="7">
+        <v>134</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C136" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="D136" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="E136" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F136" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G136" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H136" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I136" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A137" s="7">
+        <v>135</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C137" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="D137" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="E137" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F137" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G137" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H137" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I137" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A138" s="7">
+        <v>136</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C138" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="D138" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="E138" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F138" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G138" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H138" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I138" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A139" s="7">
+        <v>137</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C139" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="D139" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="E139" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F139" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G139" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H139" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I139" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A140" s="7">
+        <v>138</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C140" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="D140" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="E140" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F140" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G140" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H140" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I140" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A141" s="7">
+        <v>139</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C141" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="D141" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="E141" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F141" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G141" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H141" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I141" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A142" s="7">
+        <v>140</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C142" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="D142" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="E142" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F142" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G142" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H142" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I142" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A143" s="7">
+        <v>141</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C143" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="D143" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="E143" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F143" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G143" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H143" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I143" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A144" s="7">
+        <v>142</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C144" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="D144" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="E144" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F144" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G144" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H144" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I144" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A145" s="7">
+        <v>143</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C145" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="D145" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="E145" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F145" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G145" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H145" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I145" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A146" s="7">
+        <v>144</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C146" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="D146" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="E146" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F146" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G146" s="10">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="H146" s="14">
+        <v>45643</v>
+      </c>
+      <c r="I146" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D1:D74">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A1:I146" twoDigitTextYear="1"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated 24 december 2024
</commit_message>
<xml_diff>
--- a/Dataset/raw/12 Desember 2024.xlsx
+++ b/Dataset/raw/12 Desember 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Videos\POLYTRON\Job\Dataset\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C5AE26-04A9-4614-9BE9-EF5D85F68154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF0AD6A-6596-41A8-BA7B-0BABFEFF0F8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="baking_12_december" sheetId="2" r:id="rId1"/>
@@ -20,6 +20,8 @@
     <sheet name="baking_18" sheetId="7" r:id="rId5"/>
     <sheet name="baking_19" sheetId="9" r:id="rId6"/>
     <sheet name="baking_20" sheetId="10" r:id="rId7"/>
+    <sheet name="baking_23" sheetId="11" r:id="rId8"/>
+    <sheet name="baking_24" sheetId="12" r:id="rId9"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2885" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3483" uniqueCount="854">
   <si>
     <t>No</t>
   </si>
@@ -2134,6 +2136,465 @@
   </si>
   <si>
     <t>0KC1FKH49D303G</t>
+  </si>
+  <si>
+    <t>MF49B0271</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B3036</t>
+  </si>
+  <si>
+    <t>Not Yet</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B3034</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B3033</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B3024</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B302Q</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B302N</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B3032</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B302R</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B302S</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B3031</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B302T</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B302V</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B302W</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B3030</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B302P</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B302Z</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B302Y</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B302X</t>
+  </si>
+  <si>
+    <t>MF4990134</t>
+  </si>
+  <si>
+    <t>0KC1FKH4993014</t>
+  </si>
+  <si>
+    <t>0KC1FKH4993012</t>
+  </si>
+  <si>
+    <t>0KC1FKH4993010</t>
+  </si>
+  <si>
+    <t>0KC1FKH4993011</t>
+  </si>
+  <si>
+    <t>0KC1FKH499300Y</t>
+  </si>
+  <si>
+    <t>0KC1FKH499300X</t>
+  </si>
+  <si>
+    <t>0KC1FKH499300W</t>
+  </si>
+  <si>
+    <t>0KC1FKH499300V</t>
+  </si>
+  <si>
+    <t>0KC1FKH499300T</t>
+  </si>
+  <si>
+    <t>0KC1FKH499300S</t>
+  </si>
+  <si>
+    <t>0KC1FKH499300R</t>
+  </si>
+  <si>
+    <t>0KC1FKH499300Q</t>
+  </si>
+  <si>
+    <t>0KC1FKH499300P</t>
+  </si>
+  <si>
+    <t>0KC1FKH499300N</t>
+  </si>
+  <si>
+    <t>0KC1FKH499300M</t>
+  </si>
+  <si>
+    <t>0KC1FKH499300L</t>
+  </si>
+  <si>
+    <t>0KC1FKH499300G</t>
+  </si>
+  <si>
+    <t>0KC1FKH499300A</t>
+  </si>
+  <si>
+    <t>MF49D0187</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D303F</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D303E</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D303D</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D303C</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D303B</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D303A</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D3039</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D3038</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D3034</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D3037</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D3036</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D3035</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D3033</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D3032</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D3031</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D3030</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D302Z</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D302Y</t>
+  </si>
+  <si>
+    <t>MF49E0103</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E301N</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E301M</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E301L</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E301K</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E301J</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E301H</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E301G</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E301F</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E301D</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E301C</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E301B</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E301A</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E3019</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E3018</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E3017</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E3016</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E3015</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E3014</t>
+  </si>
+  <si>
+    <t>MF49A0238</t>
+  </si>
+  <si>
+    <t>0KC1FKH49A3027</t>
+  </si>
+  <si>
+    <t>0KC1FKH49A3042</t>
+  </si>
+  <si>
+    <t>0KC1FKH49A3041</t>
+  </si>
+  <si>
+    <t>0KC1FKH49A303Y</t>
+  </si>
+  <si>
+    <t>0KC1FKH49A303V</t>
+  </si>
+  <si>
+    <t>0KC1FKH49A303T</t>
+  </si>
+  <si>
+    <t>0KC1FKH49A303S</t>
+  </si>
+  <si>
+    <t>0KC1FKH49A303R</t>
+  </si>
+  <si>
+    <t>0KC1FKH49A303Q</t>
+  </si>
+  <si>
+    <t>0KC1FKH49A303P</t>
+  </si>
+  <si>
+    <t>0KC1FKH49A303N</t>
+  </si>
+  <si>
+    <t>0KC1FKH49A303M</t>
+  </si>
+  <si>
+    <t>0KC1FKH49A303L</t>
+  </si>
+  <si>
+    <t>0KC1FKH49A303K</t>
+  </si>
+  <si>
+    <t>0KC1FKH49A303J</t>
+  </si>
+  <si>
+    <t>0KC1FKH49A303H</t>
+  </si>
+  <si>
+    <t>0KC1FKH49A303G</t>
+  </si>
+  <si>
+    <t>0KC1FKH49A303F</t>
+  </si>
+  <si>
+    <t>MF49D0147</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D3022</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D3023</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D3020</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D301Z</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D3021</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D301Y</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D301X</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D301W</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D301V</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D302D</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D302F</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D3028</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D302A</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D302B</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D3024</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D3025</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D3026</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D3027</t>
+  </si>
+  <si>
+    <t>MF4980064</t>
+  </si>
+  <si>
+    <t>0KC1FKH498300F</t>
+  </si>
+  <si>
+    <t>0KC1FKH498300L</t>
+  </si>
+  <si>
+    <t>0KC1FKH498300K</t>
+  </si>
+  <si>
+    <t>0KC1FKH498300J</t>
+  </si>
+  <si>
+    <t>0KC1FKH498300H</t>
+  </si>
+  <si>
+    <t>0KC1FKH498300G</t>
+  </si>
+  <si>
+    <t>0KC1FKH498300E</t>
+  </si>
+  <si>
+    <t>0KC1FKH498300C</t>
+  </si>
+  <si>
+    <t>0KC1FKH498300A</t>
+  </si>
+  <si>
+    <t>0KC1FKH498300D</t>
+  </si>
+  <si>
+    <t>0KC1FKH498300B</t>
+  </si>
+  <si>
+    <t>0KC1FKH4983008</t>
+  </si>
+  <si>
+    <t>0KC1FKH4983007</t>
+  </si>
+  <si>
+    <t>0KC1FKH497303X</t>
+  </si>
+  <si>
+    <t>0KC1FKH4983006</t>
+  </si>
+  <si>
+    <t>0KC1FKH4983005</t>
+  </si>
+  <si>
+    <t>0KC1FKH4983004</t>
+  </si>
+  <si>
+    <t>0KC1FKH4983003</t>
+  </si>
+  <si>
+    <t>MF49D0003</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D3004</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D3003</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D3002</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D3001</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C3040</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C303Z</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C303Y</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C303X</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C303W</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C303V</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C303T</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C303S</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C303R</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C303Q</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C303N</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C303M</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C303L</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C303K</t>
   </si>
 </sst>
 </file>
@@ -2275,7 +2736,27 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="표준_~2585981" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4818,7 +5299,7 @@
     <mergeCell ref="D1:D2"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9077,7 +9558,7 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -13338,7 +13819,7 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D74">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -15514,7 +15995,7 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D74">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17684,7 +18165,7 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D74">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -19854,7 +20335,7 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D74">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -19864,8 +20345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F70B6AA-5825-49A8-A25A-422DAEE45532}">
   <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22024,7 +22505,4345 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D74">
-    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17257125-1BD0-4550-94C7-57FF94F3BCF1}">
+  <dimension ref="A1:I74"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="16"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>702</v>
+      </c>
+      <c r="E3" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F3" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H3" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I3" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>704</v>
+      </c>
+      <c r="E4" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F4" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H4" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>705</v>
+      </c>
+      <c r="E5" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F5" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H5" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>706</v>
+      </c>
+      <c r="E6" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F6" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H6" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I6" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>707</v>
+      </c>
+      <c r="E7" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F7" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G7" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H7" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I7" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>708</v>
+      </c>
+      <c r="E8" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F8" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G8" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H8" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I8" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>709</v>
+      </c>
+      <c r="E9" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F9" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H9" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I9" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>710</v>
+      </c>
+      <c r="E10" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F10" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H10" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I10" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>711</v>
+      </c>
+      <c r="E11" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F11" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G11" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H11" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I11" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="7">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>712</v>
+      </c>
+      <c r="E12" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F12" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H12" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>713</v>
+      </c>
+      <c r="E13" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F13" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G13" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H13" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I13" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>714</v>
+      </c>
+      <c r="E14" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F14" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G14" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H14" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I14" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="7">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>715</v>
+      </c>
+      <c r="E15" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F15" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G15" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H15" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I15" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="7">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>716</v>
+      </c>
+      <c r="E16" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F16" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G16" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H16" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I16" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="7">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>717</v>
+      </c>
+      <c r="E17" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F17" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G17" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H17" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I17" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="7">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>718</v>
+      </c>
+      <c r="E18" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F18" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G18" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H18" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I18" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="7">
+        <v>17</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>719</v>
+      </c>
+      <c r="E19" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F19" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G19" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H19" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I19" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="7">
+        <v>18</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>720</v>
+      </c>
+      <c r="E20" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F20" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G20" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H20" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I20" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="7">
+        <v>19</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>721</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>722</v>
+      </c>
+      <c r="E21" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F21" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G21" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H21" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I21" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="7">
+        <v>20</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>721</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>723</v>
+      </c>
+      <c r="E22" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F22" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G22" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H22" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I22" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="7">
+        <v>21</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>721</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>724</v>
+      </c>
+      <c r="E23" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F23" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G23" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H23" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I23" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="7">
+        <v>22</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>721</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>725</v>
+      </c>
+      <c r="E24" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F24" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G24" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H24" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I24" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="7">
+        <v>23</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>721</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>726</v>
+      </c>
+      <c r="E25" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F25" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G25" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H25" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I25" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="7">
+        <v>24</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>721</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>727</v>
+      </c>
+      <c r="E26" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F26" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G26" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H26" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I26" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="7">
+        <v>25</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>721</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>728</v>
+      </c>
+      <c r="E27" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F27" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G27" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H27" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I27" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="7">
+        <v>26</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>721</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>729</v>
+      </c>
+      <c r="E28" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F28" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G28" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H28" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I28" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="7">
+        <v>27</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>721</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>730</v>
+      </c>
+      <c r="E29" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F29" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G29" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H29" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I29" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="7">
+        <v>28</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>721</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>731</v>
+      </c>
+      <c r="E30" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F30" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G30" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H30" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I30" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="7">
+        <v>29</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>721</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>732</v>
+      </c>
+      <c r="E31" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F31" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G31" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H31" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I31" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="7">
+        <v>30</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>721</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>733</v>
+      </c>
+      <c r="E32" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F32" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G32" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H32" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I32" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="7">
+        <v>31</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>721</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>734</v>
+      </c>
+      <c r="E33" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F33" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G33" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H33" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I33" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="7">
+        <v>32</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>721</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>735</v>
+      </c>
+      <c r="E34" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F34" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G34" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H34" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I34" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="7">
+        <v>33</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>721</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>736</v>
+      </c>
+      <c r="E35" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F35" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G35" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H35" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I35" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="7">
+        <v>34</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>721</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>737</v>
+      </c>
+      <c r="E36" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F36" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G36" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H36" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I36" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="7">
+        <v>35</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>721</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>738</v>
+      </c>
+      <c r="E37" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F37" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G37" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H37" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I37" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="7">
+        <v>36</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>721</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>739</v>
+      </c>
+      <c r="E38" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F38" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G38" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H38" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I38" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="7">
+        <v>37</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>740</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>741</v>
+      </c>
+      <c r="E39" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F39" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G39" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H39" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I39" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="7">
+        <v>38</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>740</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>742</v>
+      </c>
+      <c r="E40" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F40" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G40" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H40" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I40" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="7">
+        <v>39</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>740</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>743</v>
+      </c>
+      <c r="E41" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F41" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G41" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H41" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I41" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="7">
+        <v>40</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>740</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>744</v>
+      </c>
+      <c r="E42" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F42" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G42" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H42" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I42" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="7">
+        <v>41</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>740</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>745</v>
+      </c>
+      <c r="E43" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F43" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G43" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H43" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I43" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="7">
+        <v>42</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>740</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>746</v>
+      </c>
+      <c r="E44" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F44" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G44" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H44" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I44" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="7">
+        <v>43</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>740</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>747</v>
+      </c>
+      <c r="E45" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F45" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G45" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H45" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I45" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="7">
+        <v>44</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>740</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>748</v>
+      </c>
+      <c r="E46" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F46" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G46" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H46" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I46" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="7">
+        <v>45</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>740</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>749</v>
+      </c>
+      <c r="E47" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F47" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G47" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H47" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I47" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="7">
+        <v>46</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>740</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>750</v>
+      </c>
+      <c r="E48" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F48" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G48" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H48" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I48" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="7">
+        <v>47</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>740</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>751</v>
+      </c>
+      <c r="E49" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F49" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G49" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H49" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I49" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="7">
+        <v>48</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>740</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>752</v>
+      </c>
+      <c r="E50" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F50" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G50" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H50" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I50" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="7">
+        <v>49</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>740</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>753</v>
+      </c>
+      <c r="E51" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F51" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G51" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H51" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I51" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="7">
+        <v>50</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>740</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>754</v>
+      </c>
+      <c r="E52" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F52" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G52" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H52" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I52" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="7">
+        <v>51</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>740</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>755</v>
+      </c>
+      <c r="E53" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F53" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G53" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H53" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I53" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="7">
+        <v>52</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>740</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>756</v>
+      </c>
+      <c r="E54" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F54" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G54" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H54" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I54" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="7">
+        <v>53</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>740</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>757</v>
+      </c>
+      <c r="E55" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F55" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G55" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H55" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I55" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="7">
+        <v>54</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>740</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>758</v>
+      </c>
+      <c r="E56" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F56" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G56" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H56" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I56" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="7">
+        <v>55</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>759</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>760</v>
+      </c>
+      <c r="E57" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F57" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G57" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H57" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I57" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="7">
+        <v>56</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>759</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>761</v>
+      </c>
+      <c r="E58" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F58" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G58" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H58" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I58" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="7">
+        <v>57</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>759</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>762</v>
+      </c>
+      <c r="E59" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F59" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G59" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H59" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I59" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="7">
+        <v>58</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>759</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>763</v>
+      </c>
+      <c r="E60" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F60" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G60" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H60" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I60" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="7">
+        <v>59</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>759</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>764</v>
+      </c>
+      <c r="E61" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F61" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G61" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H61" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I61" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="7">
+        <v>60</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>759</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>765</v>
+      </c>
+      <c r="E62" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F62" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G62" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H62" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I62" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="7">
+        <v>61</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>759</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>766</v>
+      </c>
+      <c r="E63" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F63" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G63" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H63" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I63" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="7">
+        <v>62</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>759</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>767</v>
+      </c>
+      <c r="E64" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F64" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G64" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H64" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I64" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="7">
+        <v>63</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>759</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>768</v>
+      </c>
+      <c r="E65" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F65" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G65" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H65" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I65" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="7">
+        <v>64</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>759</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>769</v>
+      </c>
+      <c r="E66" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F66" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G66" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H66" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I66" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="7">
+        <v>65</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>759</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>770</v>
+      </c>
+      <c r="E67" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F67" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G67" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H67" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I67" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="7">
+        <v>66</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>759</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>771</v>
+      </c>
+      <c r="E68" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F68" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G68" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H68" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I68" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="7">
+        <v>67</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>759</v>
+      </c>
+      <c r="D69" s="8" t="s">
+        <v>772</v>
+      </c>
+      <c r="E69" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F69" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G69" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H69" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I69" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="7">
+        <v>68</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>759</v>
+      </c>
+      <c r="D70" s="8" t="s">
+        <v>773</v>
+      </c>
+      <c r="E70" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F70" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G70" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H70" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I70" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="7">
+        <v>69</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>759</v>
+      </c>
+      <c r="D71" s="8" t="s">
+        <v>774</v>
+      </c>
+      <c r="E71" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F71" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G71" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H71" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I71" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="7">
+        <v>70</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C72" s="9" t="s">
+        <v>759</v>
+      </c>
+      <c r="D72" s="8" t="s">
+        <v>775</v>
+      </c>
+      <c r="E72" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F72" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G72" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H72" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I72" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="7">
+        <v>71</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>759</v>
+      </c>
+      <c r="D73" s="8" t="s">
+        <v>776</v>
+      </c>
+      <c r="E73" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F73" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G73" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H73" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I73" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="7">
+        <v>72</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>759</v>
+      </c>
+      <c r="D74" s="8" t="s">
+        <v>777</v>
+      </c>
+      <c r="E74" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F74" s="13">
+        <v>45649</v>
+      </c>
+      <c r="G74" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H74" s="13">
+        <v>45650</v>
+      </c>
+      <c r="I74" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D1:D74">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BD7668B-842D-4169-B0C5-15301A67D144}">
+  <dimension ref="A1:I74"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="7.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="16"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>778</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="E3" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F3" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>778</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>780</v>
+      </c>
+      <c r="E4" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F4" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>778</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>781</v>
+      </c>
+      <c r="E5" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F5" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>778</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>782</v>
+      </c>
+      <c r="E6" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F6" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>778</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>783</v>
+      </c>
+      <c r="E7" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F7" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G7" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>778</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>784</v>
+      </c>
+      <c r="E8" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F8" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G8" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>778</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>785</v>
+      </c>
+      <c r="E9" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F9" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>778</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="E10" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F10" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>778</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>787</v>
+      </c>
+      <c r="E11" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F11" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G11" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="7">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>778</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>788</v>
+      </c>
+      <c r="E12" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F12" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>778</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>789</v>
+      </c>
+      <c r="E13" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F13" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G13" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>778</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>790</v>
+      </c>
+      <c r="E14" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F14" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G14" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="7">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>778</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>791</v>
+      </c>
+      <c r="E15" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F15" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G15" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="7">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>778</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>792</v>
+      </c>
+      <c r="E16" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F16" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G16" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="7">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>778</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>793</v>
+      </c>
+      <c r="E17" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F17" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G17" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="7">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>778</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>794</v>
+      </c>
+      <c r="E18" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F18" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G18" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="7">
+        <v>17</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>778</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>795</v>
+      </c>
+      <c r="E19" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F19" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G19" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="7">
+        <v>18</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>778</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>796</v>
+      </c>
+      <c r="E20" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F20" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G20" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="7">
+        <v>19</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>797</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>798</v>
+      </c>
+      <c r="E21" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F21" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G21" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="7">
+        <v>20</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>797</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="E22" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F22" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G22" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="7">
+        <v>21</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>797</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>800</v>
+      </c>
+      <c r="E23" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F23" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G23" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="7">
+        <v>22</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>797</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>801</v>
+      </c>
+      <c r="E24" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F24" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G24" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I24" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="7">
+        <v>23</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>797</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>802</v>
+      </c>
+      <c r="E25" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F25" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G25" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I25" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="7">
+        <v>24</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>797</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>803</v>
+      </c>
+      <c r="E26" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F26" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G26" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I26" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="7">
+        <v>25</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>797</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>804</v>
+      </c>
+      <c r="E27" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F27" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G27" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I27" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="7">
+        <v>26</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>797</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>805</v>
+      </c>
+      <c r="E28" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F28" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G28" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I28" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="7">
+        <v>27</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>797</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>806</v>
+      </c>
+      <c r="E29" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F29" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G29" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H29" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I29" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="7">
+        <v>28</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>797</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>807</v>
+      </c>
+      <c r="E30" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F30" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G30" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I30" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="7">
+        <v>29</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>797</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>808</v>
+      </c>
+      <c r="E31" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F31" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G31" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H31" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I31" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="7">
+        <v>30</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>797</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>809</v>
+      </c>
+      <c r="E32" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F32" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G32" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I32" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="7">
+        <v>31</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>797</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>810</v>
+      </c>
+      <c r="E33" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F33" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G33" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H33" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I33" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="7">
+        <v>32</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>797</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>811</v>
+      </c>
+      <c r="E34" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F34" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G34" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H34" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I34" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="7">
+        <v>33</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>797</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>812</v>
+      </c>
+      <c r="E35" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F35" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G35" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I35" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="7">
+        <v>34</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>797</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>813</v>
+      </c>
+      <c r="E36" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F36" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G36" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H36" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I36" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="7">
+        <v>35</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>797</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>814</v>
+      </c>
+      <c r="E37" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F37" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G37" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H37" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I37" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="7">
+        <v>36</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>797</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>815</v>
+      </c>
+      <c r="E38" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F38" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G38" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H38" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I38" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="7">
+        <v>37</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>816</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>817</v>
+      </c>
+      <c r="E39" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F39" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G39" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H39" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I39" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="7">
+        <v>38</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>816</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>818</v>
+      </c>
+      <c r="E40" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F40" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G40" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H40" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I40" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="7">
+        <v>39</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>816</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>819</v>
+      </c>
+      <c r="E41" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F41" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G41" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H41" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I41" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="7">
+        <v>40</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>816</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>820</v>
+      </c>
+      <c r="E42" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F42" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G42" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H42" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I42" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="7">
+        <v>41</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>816</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>821</v>
+      </c>
+      <c r="E43" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F43" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G43" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H43" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I43" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="7">
+        <v>42</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>816</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>822</v>
+      </c>
+      <c r="E44" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F44" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G44" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H44" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I44" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="7">
+        <v>43</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>816</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>823</v>
+      </c>
+      <c r="E45" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F45" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G45" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H45" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I45" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="7">
+        <v>44</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>816</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>824</v>
+      </c>
+      <c r="E46" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F46" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G46" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H46" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I46" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="7">
+        <v>45</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>816</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>825</v>
+      </c>
+      <c r="E47" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F47" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G47" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H47" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I47" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="7">
+        <v>46</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>816</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>826</v>
+      </c>
+      <c r="E48" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F48" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G48" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H48" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I48" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="7">
+        <v>47</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>816</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>827</v>
+      </c>
+      <c r="E49" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F49" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G49" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H49" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I49" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="7">
+        <v>48</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>816</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>828</v>
+      </c>
+      <c r="E50" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F50" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G50" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H50" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I50" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="7">
+        <v>49</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>816</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>829</v>
+      </c>
+      <c r="E51" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F51" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G51" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H51" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I51" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="7">
+        <v>50</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>816</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>830</v>
+      </c>
+      <c r="E52" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F52" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G52" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H52" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I52" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="7">
+        <v>51</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>816</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>831</v>
+      </c>
+      <c r="E53" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F53" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G53" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H53" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I53" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="7">
+        <v>52</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>816</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>832</v>
+      </c>
+      <c r="E54" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F54" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G54" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H54" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I54" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="7">
+        <v>53</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>816</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>833</v>
+      </c>
+      <c r="E55" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F55" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G55" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H55" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I55" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="7">
+        <v>54</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>816</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>834</v>
+      </c>
+      <c r="E56" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F56" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G56" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H56" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I56" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="7">
+        <v>55</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>835</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>836</v>
+      </c>
+      <c r="E57" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F57" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G57" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H57" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I57" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="7">
+        <v>56</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>835</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>837</v>
+      </c>
+      <c r="E58" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F58" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G58" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H58" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I58" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="7">
+        <v>57</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>835</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>838</v>
+      </c>
+      <c r="E59" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F59" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G59" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H59" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I59" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="7">
+        <v>58</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>835</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>839</v>
+      </c>
+      <c r="E60" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F60" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G60" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H60" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I60" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="7">
+        <v>59</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>835</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>840</v>
+      </c>
+      <c r="E61" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F61" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G61" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H61" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I61" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="7">
+        <v>60</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>835</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>841</v>
+      </c>
+      <c r="E62" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F62" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G62" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H62" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I62" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="7">
+        <v>61</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>835</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>842</v>
+      </c>
+      <c r="E63" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F63" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G63" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H63" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I63" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="7">
+        <v>62</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>835</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>843</v>
+      </c>
+      <c r="E64" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F64" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G64" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H64" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I64" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="7">
+        <v>63</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>835</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>844</v>
+      </c>
+      <c r="E65" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F65" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G65" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H65" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I65" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="7">
+        <v>64</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>835</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>845</v>
+      </c>
+      <c r="E66" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F66" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G66" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H66" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I66" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="7">
+        <v>65</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>835</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>846</v>
+      </c>
+      <c r="E67" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F67" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G67" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H67" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I67" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="7">
+        <v>66</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>835</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>847</v>
+      </c>
+      <c r="E68" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F68" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G68" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H68" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I68" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="7">
+        <v>67</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>835</v>
+      </c>
+      <c r="D69" s="8" t="s">
+        <v>848</v>
+      </c>
+      <c r="E69" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F69" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G69" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H69" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I69" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="7">
+        <v>68</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>835</v>
+      </c>
+      <c r="D70" s="8" t="s">
+        <v>849</v>
+      </c>
+      <c r="E70" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F70" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G70" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H70" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I70" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="7">
+        <v>69</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>835</v>
+      </c>
+      <c r="D71" s="8" t="s">
+        <v>850</v>
+      </c>
+      <c r="E71" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F71" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G71" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H71" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I71" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="7">
+        <v>70</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C72" s="9" t="s">
+        <v>835</v>
+      </c>
+      <c r="D72" s="8" t="s">
+        <v>851</v>
+      </c>
+      <c r="E72" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F72" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G72" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H72" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I72" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="7">
+        <v>71</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>835</v>
+      </c>
+      <c r="D73" s="8" t="s">
+        <v>852</v>
+      </c>
+      <c r="E73" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F73" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G73" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H73" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I73" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="7">
+        <v>72</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>835</v>
+      </c>
+      <c r="D74" s="8" t="s">
+        <v>853</v>
+      </c>
+      <c r="E74" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F74" s="13">
+        <v>45650</v>
+      </c>
+      <c r="G74" s="6">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H74" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="I74" s="13" t="s">
+        <v>703</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D1:D74">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated 02 jan 2025
</commit_message>
<xml_diff>
--- a/Dataset/raw/12 Desember 2024.xlsx
+++ b/Dataset/raw/12 Desember 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Videos\POLYTRON\Job\Dataset\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBBA8D54-33CC-4BF0-8884-6A95F6542704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94378449-8D97-4CD8-A779-19D1B5ABEE74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="6" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="baking_12_december" sheetId="2" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="baking_27" sheetId="15" r:id="rId11"/>
     <sheet name="baking_30" sheetId="17" r:id="rId12"/>
     <sheet name="baking_31" sheetId="19" r:id="rId13"/>
+    <sheet name="baking_02_jan" sheetId="20" r:id="rId14"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4391" uniqueCount="1158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4618" uniqueCount="1234">
   <si>
     <t>No</t>
   </si>
@@ -3511,6 +3512,234 @@
   </si>
   <si>
     <t>0KC1FKH49C301X</t>
+  </si>
+  <si>
+    <t>MF49D0029</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D300N</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D300M</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D300L</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D300K</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D300J</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D300H</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D300G</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D300F</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D300E</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D300D</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D300C</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D300B</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D300A</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D3009</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D3008</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D3007</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D3005</t>
+  </si>
+  <si>
+    <t>0KC1FKH49D3006</t>
+  </si>
+  <si>
+    <t>MF49C0001</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B303F</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B303E</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B303D</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B303C</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B303B</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B303A</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B3039</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B3038</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B3037</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C3002</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C3001</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B303N</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B303K</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B303L</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B303J</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B303M</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B303H</t>
+  </si>
+  <si>
+    <t>0KC1FKH49B303G</t>
+  </si>
+  <si>
+    <t>MF49E0100</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E300T</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E300W</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E300V</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E300Y</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E300X</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E3010</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E300Z</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E3013</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E3011</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E300J</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E300L</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E300K</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E300N</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E300M</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E300Q</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E300P</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E300S</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E300R</t>
+  </si>
+  <si>
+    <t>MF49E0132</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E302H</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E302G</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E302F</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E302E</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E302D</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E302B</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E3028</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E3029</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E302A</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E302S</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E302R</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E302Q</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E302P</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E302N</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E302M</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E302L</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E302K</t>
+  </si>
+  <si>
+    <t>0KC1FKH49E302J</t>
   </si>
 </sst>
 </file>
@@ -3616,7 +3845,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3661,12 +3890,38 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="표준_~2585981" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -6299,7 +6554,7 @@
     <mergeCell ref="D1:D2"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="duplicateValues" dxfId="15" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8470,7 +8725,7 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D74">
-    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10640,10 +10895,10 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D2">
-    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D74">
-    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12885,10 +13140,10 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D2">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D74">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12898,8 +13153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD158DEB-B13F-4620-825A-80F609EA3C62}">
   <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12981,11 +13236,11 @@
       <c r="G3" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H3" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>1007</v>
+      <c r="H3" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I3" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -13010,11 +13265,11 @@
       <c r="G4" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H4" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I4" s="13" t="s">
-        <v>1007</v>
+      <c r="H4" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I4" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -13039,11 +13294,11 @@
       <c r="G5" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H5" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>1007</v>
+      <c r="H5" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I5" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -13068,11 +13323,11 @@
       <c r="G6" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H6" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I6" s="13" t="s">
-        <v>1007</v>
+      <c r="H6" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I6" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -13097,11 +13352,11 @@
       <c r="G7" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H7" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I7" s="13" t="s">
-        <v>1007</v>
+      <c r="H7" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I7" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -13126,11 +13381,11 @@
       <c r="G8" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H8" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I8" s="13" t="s">
-        <v>1007</v>
+      <c r="H8" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I8" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -13155,11 +13410,11 @@
       <c r="G9" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H9" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I9" s="13" t="s">
-        <v>1007</v>
+      <c r="H9" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I9" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -13184,11 +13439,11 @@
       <c r="G10" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H10" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>1007</v>
+      <c r="H10" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I10" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -13213,11 +13468,11 @@
       <c r="G11" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H11" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I11" s="13" t="s">
-        <v>1007</v>
+      <c r="H11" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I11" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -13242,11 +13497,11 @@
       <c r="G12" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H12" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>1007</v>
+      <c r="H12" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I12" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -13271,11 +13526,11 @@
       <c r="G13" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H13" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I13" s="13" t="s">
-        <v>1007</v>
+      <c r="H13" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I13" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -13300,11 +13555,11 @@
       <c r="G14" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H14" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I14" s="13" t="s">
-        <v>1007</v>
+      <c r="H14" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I14" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -13329,11 +13584,11 @@
       <c r="G15" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H15" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I15" s="13" t="s">
-        <v>1007</v>
+      <c r="H15" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I15" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -13358,11 +13613,11 @@
       <c r="G16" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H16" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I16" s="13" t="s">
-        <v>1007</v>
+      <c r="H16" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I16" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -13387,11 +13642,11 @@
       <c r="G17" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H17" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I17" s="13" t="s">
-        <v>1007</v>
+      <c r="H17" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I17" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -13416,11 +13671,11 @@
       <c r="G18" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H18" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I18" s="13" t="s">
-        <v>1007</v>
+      <c r="H18" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I18" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -13445,11 +13700,11 @@
       <c r="G19" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H19" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I19" s="13" t="s">
-        <v>1007</v>
+      <c r="H19" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I19" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -13474,11 +13729,11 @@
       <c r="G20" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H20" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I20" s="13" t="s">
-        <v>1007</v>
+      <c r="H20" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I20" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -13503,11 +13758,11 @@
       <c r="G21" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H21" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I21" s="13" t="s">
-        <v>1007</v>
+      <c r="H21" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I21" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -13532,11 +13787,11 @@
       <c r="G22" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H22" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I22" s="13" t="s">
-        <v>1007</v>
+      <c r="H22" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I22" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -13561,11 +13816,11 @@
       <c r="G23" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H23" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I23" s="13" t="s">
-        <v>1007</v>
+      <c r="H23" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I23" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -13590,11 +13845,11 @@
       <c r="G24" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H24" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I24" s="13" t="s">
-        <v>1007</v>
+      <c r="H24" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I24" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -13619,11 +13874,11 @@
       <c r="G25" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H25" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I25" s="13" t="s">
-        <v>1007</v>
+      <c r="H25" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I25" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -13648,11 +13903,11 @@
       <c r="G26" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H26" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I26" s="13" t="s">
-        <v>1007</v>
+      <c r="H26" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I26" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -13677,11 +13932,11 @@
       <c r="G27" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H27" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I27" s="13" t="s">
-        <v>1007</v>
+      <c r="H27" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I27" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -13706,11 +13961,11 @@
       <c r="G28" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H28" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I28" s="13" t="s">
-        <v>1007</v>
+      <c r="H28" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I28" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -13735,11 +13990,11 @@
       <c r="G29" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H29" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I29" s="13" t="s">
-        <v>1007</v>
+      <c r="H29" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I29" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -13764,11 +14019,11 @@
       <c r="G30" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H30" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I30" s="13" t="s">
-        <v>1007</v>
+      <c r="H30" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I30" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -13793,11 +14048,11 @@
       <c r="G31" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H31" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I31" s="13" t="s">
-        <v>1007</v>
+      <c r="H31" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I31" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -13822,11 +14077,11 @@
       <c r="G32" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H32" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I32" s="13" t="s">
-        <v>1007</v>
+      <c r="H32" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I32" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -13851,11 +14106,11 @@
       <c r="G33" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H33" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I33" s="13" t="s">
-        <v>1007</v>
+      <c r="H33" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I33" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -13880,11 +14135,11 @@
       <c r="G34" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H34" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I34" s="13" t="s">
-        <v>1007</v>
+      <c r="H34" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I34" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -13909,11 +14164,11 @@
       <c r="G35" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H35" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I35" s="13" t="s">
-        <v>1007</v>
+      <c r="H35" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I35" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -13938,11 +14193,11 @@
       <c r="G36" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H36" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I36" s="13" t="s">
-        <v>1007</v>
+      <c r="H36" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I36" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -13967,11 +14222,11 @@
       <c r="G37" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H37" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I37" s="13" t="s">
-        <v>1007</v>
+      <c r="H37" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I37" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -13996,11 +14251,11 @@
       <c r="G38" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H38" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I38" s="13" t="s">
-        <v>1007</v>
+      <c r="H38" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I38" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -14025,11 +14280,11 @@
       <c r="G39" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H39" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I39" s="13" t="s">
-        <v>1007</v>
+      <c r="H39" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I39" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -14054,11 +14309,11 @@
       <c r="G40" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H40" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I40" s="13" t="s">
-        <v>1007</v>
+      <c r="H40" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I40" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -14083,11 +14338,11 @@
       <c r="G41" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H41" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I41" s="13" t="s">
-        <v>1007</v>
+      <c r="H41" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I41" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -14112,11 +14367,11 @@
       <c r="G42" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H42" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I42" s="13" t="s">
-        <v>1007</v>
+      <c r="H42" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I42" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -14141,11 +14396,11 @@
       <c r="G43" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H43" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I43" s="13" t="s">
-        <v>1007</v>
+      <c r="H43" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I43" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -14170,11 +14425,11 @@
       <c r="G44" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H44" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I44" s="13" t="s">
-        <v>1007</v>
+      <c r="H44" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I44" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -14199,11 +14454,11 @@
       <c r="G45" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H45" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I45" s="13" t="s">
-        <v>1007</v>
+      <c r="H45" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I45" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -14228,11 +14483,11 @@
       <c r="G46" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H46" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I46" s="13" t="s">
-        <v>1007</v>
+      <c r="H46" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I46" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -14257,11 +14512,11 @@
       <c r="G47" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H47" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I47" s="13" t="s">
-        <v>1007</v>
+      <c r="H47" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I47" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -14286,11 +14541,11 @@
       <c r="G48" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H48" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I48" s="13" t="s">
-        <v>1007</v>
+      <c r="H48" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I48" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -14315,11 +14570,11 @@
       <c r="G49" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H49" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I49" s="13" t="s">
-        <v>1007</v>
+      <c r="H49" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I49" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -14344,11 +14599,11 @@
       <c r="G50" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H50" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I50" s="13" t="s">
-        <v>1007</v>
+      <c r="H50" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I50" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -14373,11 +14628,11 @@
       <c r="G51" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H51" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I51" s="13" t="s">
-        <v>1007</v>
+      <c r="H51" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I51" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -14402,11 +14657,11 @@
       <c r="G52" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H52" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I52" s="13" t="s">
-        <v>1007</v>
+      <c r="H52" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I52" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -14431,11 +14686,11 @@
       <c r="G53" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H53" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I53" s="13" t="s">
-        <v>1007</v>
+      <c r="H53" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I53" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -14460,11 +14715,11 @@
       <c r="G54" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H54" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I54" s="13" t="s">
-        <v>1007</v>
+      <c r="H54" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I54" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -14489,11 +14744,11 @@
       <c r="G55" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H55" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I55" s="13" t="s">
-        <v>1007</v>
+      <c r="H55" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I55" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -14518,11 +14773,11 @@
       <c r="G56" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H56" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I56" s="13" t="s">
-        <v>1007</v>
+      <c r="H56" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I56" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -14547,11 +14802,11 @@
       <c r="G57" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H57" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I57" s="13" t="s">
-        <v>1007</v>
+      <c r="H57" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I57" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -14576,11 +14831,11 @@
       <c r="G58" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H58" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I58" s="13" t="s">
-        <v>1007</v>
+      <c r="H58" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I58" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -14605,11 +14860,11 @@
       <c r="G59" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H59" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I59" s="13" t="s">
-        <v>1007</v>
+      <c r="H59" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I59" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -14634,11 +14889,11 @@
       <c r="G60" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H60" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I60" s="13" t="s">
-        <v>1007</v>
+      <c r="H60" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I60" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -14663,11 +14918,11 @@
       <c r="G61" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H61" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I61" s="13" t="s">
-        <v>1007</v>
+      <c r="H61" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I61" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -14692,11 +14947,11 @@
       <c r="G62" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H62" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I62" s="13" t="s">
-        <v>1007</v>
+      <c r="H62" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I62" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -14721,11 +14976,11 @@
       <c r="G63" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H63" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I63" s="13" t="s">
-        <v>1007</v>
+      <c r="H63" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I63" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -14750,11 +15005,11 @@
       <c r="G64" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H64" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I64" s="13" t="s">
-        <v>1007</v>
+      <c r="H64" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I64" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -14779,11 +15034,11 @@
       <c r="G65" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H65" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I65" s="13" t="s">
-        <v>1007</v>
+      <c r="H65" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I65" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -14808,11 +15063,11 @@
       <c r="G66" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H66" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I66" s="13" t="s">
-        <v>1007</v>
+      <c r="H66" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I66" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -14837,11 +15092,11 @@
       <c r="G67" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H67" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I67" s="13" t="s">
-        <v>1007</v>
+      <c r="H67" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I67" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -14866,11 +15121,11 @@
       <c r="G68" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H68" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I68" s="13" t="s">
-        <v>1007</v>
+      <c r="H68" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I68" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -14895,11 +15150,11 @@
       <c r="G69" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H69" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I69" s="13" t="s">
-        <v>1007</v>
+      <c r="H69" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I69" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -14924,11 +15179,11 @@
       <c r="G70" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H70" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I70" s="13" t="s">
-        <v>1007</v>
+      <c r="H70" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I70" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -14953,11 +15208,11 @@
       <c r="G71" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H71" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I71" s="13" t="s">
-        <v>1007</v>
+      <c r="H71" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I71" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -14982,11 +15237,11 @@
       <c r="G72" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H72" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I72" s="13" t="s">
-        <v>1007</v>
+      <c r="H72" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I72" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -15011,11 +15266,11 @@
       <c r="G73" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H73" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I73" s="13" t="s">
-        <v>1007</v>
+      <c r="H73" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I73" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -15040,11 +15295,11 @@
       <c r="G74" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H74" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I74" s="13" t="s">
-        <v>1007</v>
+      <c r="H74" s="18">
+        <v>45659</v>
+      </c>
+      <c r="I74" s="19">
+        <v>0.41666666666666669</v>
       </c>
     </row>
   </sheetData>
@@ -15058,10 +15313,2183 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D2">
-    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D74">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5113C119-7BB4-4304-A88E-D0533852E833}">
+  <dimension ref="A1:I74"/>
+  <sheetViews>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3:G74"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="17"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>1158</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>1159</v>
+      </c>
+      <c r="E3" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F3" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>1158</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>1160</v>
+      </c>
+      <c r="E4" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F4" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I4" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>1158</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>1161</v>
+      </c>
+      <c r="E5" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F5" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>1158</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>1162</v>
+      </c>
+      <c r="E6" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F6" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>1158</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>1163</v>
+      </c>
+      <c r="E7" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F7" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G7" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>1158</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>1164</v>
+      </c>
+      <c r="E8" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F8" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G8" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I8" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>1158</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E9" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F9" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I9" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>1158</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>1166</v>
+      </c>
+      <c r="E10" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F10" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H10" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I10" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>1158</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>1167</v>
+      </c>
+      <c r="E11" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F11" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G11" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I11" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>1158</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>1168</v>
+      </c>
+      <c r="E12" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F12" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I12" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>1158</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>1169</v>
+      </c>
+      <c r="E13" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F13" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G13" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H13" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I13" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>1158</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>1170</v>
+      </c>
+      <c r="E14" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F14" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G14" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H14" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I14" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>1158</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>1171</v>
+      </c>
+      <c r="E15" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F15" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G15" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H15" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I15" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>1158</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>1172</v>
+      </c>
+      <c r="E16" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F16" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G16" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H16" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I16" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>1158</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>1173</v>
+      </c>
+      <c r="E17" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F17" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G17" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H17" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I17" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>1158</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>1174</v>
+      </c>
+      <c r="E18" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F18" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G18" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H18" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I18" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>17</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>1158</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E19" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F19" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G19" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H19" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I19" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>18</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>1158</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>1176</v>
+      </c>
+      <c r="E20" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F20" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G20" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H20" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I20" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>19</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>1178</v>
+      </c>
+      <c r="E21" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F21" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G21" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H21" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I21" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>20</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>1179</v>
+      </c>
+      <c r="E22" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F22" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G22" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H22" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I22" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>21</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>1180</v>
+      </c>
+      <c r="E23" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F23" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G23" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H23" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I23" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>22</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>1181</v>
+      </c>
+      <c r="E24" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F24" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G24" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H24" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I24" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>23</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>1182</v>
+      </c>
+      <c r="E25" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F25" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G25" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H25" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I25" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>24</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>1183</v>
+      </c>
+      <c r="E26" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F26" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G26" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H26" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I26" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>25</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>1184</v>
+      </c>
+      <c r="E27" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F27" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G27" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H27" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I27" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>26</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>1185</v>
+      </c>
+      <c r="E28" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F28" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G28" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H28" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I28" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>27</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>1186</v>
+      </c>
+      <c r="E29" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F29" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G29" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H29" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I29" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>28</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>1187</v>
+      </c>
+      <c r="E30" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F30" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G30" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H30" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I30" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <v>29</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>1188</v>
+      </c>
+      <c r="E31" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F31" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G31" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H31" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I31" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <v>30</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>1189</v>
+      </c>
+      <c r="E32" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F32" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G32" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H32" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I32" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
+        <v>31</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>1190</v>
+      </c>
+      <c r="E33" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F33" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G33" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H33" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I33" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
+        <v>32</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>1191</v>
+      </c>
+      <c r="E34" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F34" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G34" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H34" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I34" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
+        <v>33</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>1192</v>
+      </c>
+      <c r="E35" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F35" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G35" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H35" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I35" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
+        <v>34</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>1193</v>
+      </c>
+      <c r="E36" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F36" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G36" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H36" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I36" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
+        <v>35</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>1194</v>
+      </c>
+      <c r="E37" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F37" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G37" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H37" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I37" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="2">
+        <v>36</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>1195</v>
+      </c>
+      <c r="E38" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F38" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G38" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H38" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I38" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
+        <v>37</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>1197</v>
+      </c>
+      <c r="E39" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F39" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G39" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H39" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I39" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="2">
+        <v>38</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>1198</v>
+      </c>
+      <c r="E40" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F40" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G40" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H40" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I40" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="2">
+        <v>39</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>1199</v>
+      </c>
+      <c r="E41" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F41" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G41" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H41" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I41" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="2">
+        <v>40</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>1200</v>
+      </c>
+      <c r="E42" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F42" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G42" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H42" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I42" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="2">
+        <v>41</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>1201</v>
+      </c>
+      <c r="E43" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F43" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G43" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H43" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I43" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="2">
+        <v>42</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>1202</v>
+      </c>
+      <c r="E44" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F44" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G44" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H44" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I44" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="2">
+        <v>43</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>1203</v>
+      </c>
+      <c r="E45" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F45" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G45" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H45" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I45" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="2">
+        <v>44</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>1204</v>
+      </c>
+      <c r="E46" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F46" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G46" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H46" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I46" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="2">
+        <v>45</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>1205</v>
+      </c>
+      <c r="E47" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F47" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G47" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H47" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I47" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="2">
+        <v>46</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>1206</v>
+      </c>
+      <c r="E48" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F48" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G48" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H48" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I48" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="2">
+        <v>47</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>1207</v>
+      </c>
+      <c r="E49" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F49" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G49" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H49" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I49" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="2">
+        <v>48</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>1208</v>
+      </c>
+      <c r="E50" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F50" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G50" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H50" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I50" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="2">
+        <v>49</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>1209</v>
+      </c>
+      <c r="E51" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F51" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G51" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H51" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I51" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="2">
+        <v>50</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>1210</v>
+      </c>
+      <c r="E52" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F52" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G52" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H52" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I52" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="2">
+        <v>51</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>1211</v>
+      </c>
+      <c r="E53" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F53" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G53" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H53" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I53" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="2">
+        <v>52</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>1212</v>
+      </c>
+      <c r="E54" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F54" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G54" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H54" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I54" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="2">
+        <v>53</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>1213</v>
+      </c>
+      <c r="E55" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F55" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G55" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H55" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I55" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="2">
+        <v>54</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>1214</v>
+      </c>
+      <c r="E56" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F56" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G56" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H56" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I56" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="2">
+        <v>55</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D57" s="16" t="s">
+        <v>1216</v>
+      </c>
+      <c r="E57" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F57" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G57" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H57" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I57" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="2">
+        <v>56</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>1217</v>
+      </c>
+      <c r="E58" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F58" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G58" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H58" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I58" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="2">
+        <v>57</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>1218</v>
+      </c>
+      <c r="E59" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F59" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G59" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H59" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I59" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="2">
+        <v>58</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>1219</v>
+      </c>
+      <c r="E60" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F60" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G60" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H60" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I60" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="2">
+        <v>59</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>1220</v>
+      </c>
+      <c r="E61" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F61" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G61" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H61" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I61" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="2">
+        <v>60</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>1221</v>
+      </c>
+      <c r="E62" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F62" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G62" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H62" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I62" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="2">
+        <v>61</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>1222</v>
+      </c>
+      <c r="E63" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F63" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G63" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H63" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I63" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="2">
+        <v>62</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>1223</v>
+      </c>
+      <c r="E64" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F64" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G64" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H64" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I64" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="2">
+        <v>63</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>1224</v>
+      </c>
+      <c r="E65" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F65" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G65" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H65" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I65" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="2">
+        <v>64</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>1225</v>
+      </c>
+      <c r="E66" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F66" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G66" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H66" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I66" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="2">
+        <v>65</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>1226</v>
+      </c>
+      <c r="E67" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F67" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G67" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H67" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I67" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="2">
+        <v>66</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>1227</v>
+      </c>
+      <c r="E68" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F68" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G68" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H68" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I68" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="2">
+        <v>67</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D69" s="8" t="s">
+        <v>1228</v>
+      </c>
+      <c r="E69" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F69" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G69" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H69" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I69" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="2">
+        <v>68</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D70" s="8" t="s">
+        <v>1229</v>
+      </c>
+      <c r="E70" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F70" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G70" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H70" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I70" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="2">
+        <v>69</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D71" s="8" t="s">
+        <v>1230</v>
+      </c>
+      <c r="E71" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F71" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G71" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H71" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I71" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="2">
+        <v>70</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C72" s="9" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D72" s="8" t="s">
+        <v>1231</v>
+      </c>
+      <c r="E72" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F72" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G72" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H72" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I72" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="2">
+        <v>71</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D73" s="8" t="s">
+        <v>1232</v>
+      </c>
+      <c r="E73" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F73" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G73" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H73" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I73" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="2">
+        <v>72</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D74" s="8" t="s">
+        <v>1233</v>
+      </c>
+      <c r="E74" s="4">
+        <v>801983371</v>
+      </c>
+      <c r="F74" s="13">
+        <v>45659</v>
+      </c>
+      <c r="G74" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="H74" s="18" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I74" s="19" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D1:D2">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D74">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -19319,7 +21747,7 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="duplicateValues" dxfId="14" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -23580,7 +26008,7 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D74">
-    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -25756,7 +28184,7 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D74">
-    <cfRule type="duplicateValues" dxfId="12" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -27926,7 +30354,7 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D74">
-    <cfRule type="duplicateValues" dxfId="11" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -27936,7 +30364,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{478E4E42-F398-4C65-BF3C-2DE2ABC0E541}">
   <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+    <sheetView topLeftCell="A51" workbookViewId="0">
       <selection activeCell="H76" sqref="H76"/>
     </sheetView>
   </sheetViews>
@@ -30096,7 +32524,7 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D74">
-    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -32266,7 +34694,7 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D74">
-    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -34435,7 +36863,7 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D74">
-    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -36605,7 +39033,7 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D74">
-    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated 3 january 2025
</commit_message>
<xml_diff>
--- a/Dataset/raw/12 Desember 2024.xlsx
+++ b/Dataset/raw/12 Desember 2024.xlsx
@@ -8,25 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Videos\POLYTRON\Job\Dataset\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94378449-8D97-4CD8-A779-19D1B5ABEE74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438F402D-7AEA-4E01-BD73-1A787DF6FB9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="6" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="7" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="baking_12_december" sheetId="2" r:id="rId1"/>
-    <sheet name="baking_13" sheetId="3" r:id="rId2"/>
-    <sheet name="baking_16" sheetId="4" r:id="rId3"/>
-    <sheet name="baking_17" sheetId="5" r:id="rId4"/>
-    <sheet name="baking_18" sheetId="7" r:id="rId5"/>
-    <sheet name="baking_19" sheetId="9" r:id="rId6"/>
-    <sheet name="baking_20" sheetId="10" r:id="rId7"/>
-    <sheet name="baking_23" sheetId="11" r:id="rId8"/>
-    <sheet name="baking_24" sheetId="12" r:id="rId9"/>
-    <sheet name="baking_26" sheetId="14" r:id="rId10"/>
-    <sheet name="baking_27" sheetId="15" r:id="rId11"/>
-    <sheet name="baking_30" sheetId="17" r:id="rId12"/>
-    <sheet name="baking_31" sheetId="19" r:id="rId13"/>
-    <sheet name="baking_02_jan" sheetId="20" r:id="rId14"/>
+    <sheet name="12-12-24" sheetId="2" r:id="rId1"/>
+    <sheet name="13-12-24" sheetId="3" r:id="rId2"/>
+    <sheet name="16-12-24" sheetId="4" r:id="rId3"/>
+    <sheet name="17-12-24" sheetId="5" r:id="rId4"/>
+    <sheet name="18-12-24" sheetId="7" r:id="rId5"/>
+    <sheet name="19-12-24" sheetId="9" r:id="rId6"/>
+    <sheet name="20-12-24" sheetId="10" r:id="rId7"/>
+    <sheet name="21-12-24" sheetId="11" r:id="rId8"/>
+    <sheet name="24-12-24" sheetId="12" r:id="rId9"/>
+    <sheet name="26-12-24" sheetId="14" r:id="rId10"/>
+    <sheet name="27-12-24" sheetId="15" r:id="rId11"/>
+    <sheet name="30-12-24" sheetId="17" r:id="rId12"/>
+    <sheet name="31-12-24" sheetId="19" r:id="rId13"/>
+    <sheet name="02-01-25" sheetId="20" r:id="rId14"/>
+    <sheet name="03-01-25" sheetId="22" r:id="rId15"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4618" uniqueCount="1234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4845" uniqueCount="1310">
   <si>
     <t>No</t>
   </si>
@@ -3740,6 +3741,234 @@
   </si>
   <si>
     <t>0KC1FKH49E302J</t>
+  </si>
+  <si>
+    <t>MF49C0012</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C3003</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C3004</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C3005</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C3006</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C3007</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C3008</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C3009</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C300A</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C300B</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C300C</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C300D</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C300E</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C300F</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C300G</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C300J</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C300K</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C300L</t>
+  </si>
+  <si>
+    <t>0KC1FKH49C300M</t>
+  </si>
+  <si>
+    <t>MF49F0062</t>
+  </si>
+  <si>
+    <t>0KC1FKH497303H</t>
+  </si>
+  <si>
+    <t>0KC1FKH49F300J</t>
+  </si>
+  <si>
+    <t>0KC1FKH49F3009</t>
+  </si>
+  <si>
+    <t>0KC1FKH49F3008</t>
+  </si>
+  <si>
+    <t>0KC1FKH49F3006</t>
+  </si>
+  <si>
+    <t>0KC1FKH49F3005</t>
+  </si>
+  <si>
+    <t>0KC1FKH49F3003</t>
+  </si>
+  <si>
+    <t>0KC1FKH49F3002</t>
+  </si>
+  <si>
+    <t>0KC1FKH49F3001</t>
+  </si>
+  <si>
+    <t>0KC1FKH497303F</t>
+  </si>
+  <si>
+    <t>0KC1FKH49F300H</t>
+  </si>
+  <si>
+    <t>0KC1FKH49F300G</t>
+  </si>
+  <si>
+    <t>0KC1FKH49F300F</t>
+  </si>
+  <si>
+    <t>0KC1FKH49F300E</t>
+  </si>
+  <si>
+    <t>0KC1FKH49F300D</t>
+  </si>
+  <si>
+    <t>0KC1FKH49F300C</t>
+  </si>
+  <si>
+    <t>0KC1FKH49F300B</t>
+  </si>
+  <si>
+    <t>0KC1FKH49F300A</t>
+  </si>
+  <si>
+    <t>MF4970266</t>
+  </si>
+  <si>
+    <t>0KC1FKH4973030</t>
+  </si>
+  <si>
+    <t>0KC1FKH497302X</t>
+  </si>
+  <si>
+    <t>0KC1FKH4973033</t>
+  </si>
+  <si>
+    <t>0KC1FKH4973036</t>
+  </si>
+  <si>
+    <t>0KC1FKH497303B</t>
+  </si>
+  <si>
+    <t>0KC1FKH497303A</t>
+  </si>
+  <si>
+    <t>0KC1FKH497303C</t>
+  </si>
+  <si>
+    <t>0KC1FKH4973039</t>
+  </si>
+  <si>
+    <t>0KC1FKH4973038</t>
+  </si>
+  <si>
+    <t>0HC1F584AG3006</t>
+  </si>
+  <si>
+    <t>0HC1F584AG3004</t>
+  </si>
+  <si>
+    <t>0KC1FKH49F3004</t>
+  </si>
+  <si>
+    <t>0KC1FKH49F3007</t>
+  </si>
+  <si>
+    <t>0KC1FKH4973037</t>
+  </si>
+  <si>
+    <t>0KC1FKH4973034</t>
+  </si>
+  <si>
+    <t>0KC1FKH4973035</t>
+  </si>
+  <si>
+    <t>0KC1FKH497303E</t>
+  </si>
+  <si>
+    <t>0KC1FKH497302Y</t>
+  </si>
+  <si>
+    <t>MF49G0263</t>
+  </si>
+  <si>
+    <t>0KC1FKH49G303L</t>
+  </si>
+  <si>
+    <t>0KC1FKH49G303K</t>
+  </si>
+  <si>
+    <t>0KC1FKH49G303J</t>
+  </si>
+  <si>
+    <t>0KC1FKH49G303H</t>
+  </si>
+  <si>
+    <t>0KC1FKH49G303G</t>
+  </si>
+  <si>
+    <t>0KC1FKH49G303F</t>
+  </si>
+  <si>
+    <t>0KC1FKH49G303E</t>
+  </si>
+  <si>
+    <t>0KC1FKH49G303D</t>
+  </si>
+  <si>
+    <t>0KC1FKH49G301J</t>
+  </si>
+  <si>
+    <t>0KC1FKH49G303W</t>
+  </si>
+  <si>
+    <t>0KC1FKH49G303V</t>
+  </si>
+  <si>
+    <t>0KC1FKH49G303T</t>
+  </si>
+  <si>
+    <t>0KC1FKH49G303S</t>
+  </si>
+  <si>
+    <t>0KC1FKH49G303R</t>
+  </si>
+  <si>
+    <t>0KC1FKH49G303Q</t>
+  </si>
+  <si>
+    <t>0KC1FKH49G303P</t>
+  </si>
+  <si>
+    <t>0KC1FKH49G303N</t>
+  </si>
+  <si>
+    <t>0KC1FKH49G303M</t>
   </si>
 </sst>
 </file>
@@ -3845,7 +4074,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3890,6 +4119,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3901,7 +4133,97 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="표준_~2585981" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="27">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -6554,7 +6876,7 @@
     <mergeCell ref="D1:D2"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="duplicateValues" dxfId="17" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8725,7 +9047,7 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D74">
-    <cfRule type="duplicateValues" dxfId="8" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10895,10 +11217,10 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D2">
-    <cfRule type="duplicateValues" dxfId="7" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D74">
-    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13140,10 +13462,10 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D2">
-    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D74">
-    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13153,7 +13475,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD158DEB-B13F-4620-825A-80F609EA3C62}">
   <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
@@ -13236,10 +13558,10 @@
       <c r="G3" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H3" s="18">
+      <c r="H3" s="13">
         <v>45659</v>
       </c>
-      <c r="I3" s="19">
+      <c r="I3" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -13265,10 +13587,10 @@
       <c r="G4" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H4" s="18">
+      <c r="H4" s="13">
         <v>45659</v>
       </c>
-      <c r="I4" s="19">
+      <c r="I4" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -13294,10 +13616,10 @@
       <c r="G5" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H5" s="18">
+      <c r="H5" s="13">
         <v>45659</v>
       </c>
-      <c r="I5" s="19">
+      <c r="I5" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -13323,10 +13645,10 @@
       <c r="G6" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H6" s="18">
+      <c r="H6" s="13">
         <v>45659</v>
       </c>
-      <c r="I6" s="19">
+      <c r="I6" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -13352,10 +13674,10 @@
       <c r="G7" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H7" s="18">
+      <c r="H7" s="13">
         <v>45659</v>
       </c>
-      <c r="I7" s="19">
+      <c r="I7" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -13381,10 +13703,10 @@
       <c r="G8" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H8" s="18">
+      <c r="H8" s="13">
         <v>45659</v>
       </c>
-      <c r="I8" s="19">
+      <c r="I8" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -13410,10 +13732,10 @@
       <c r="G9" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H9" s="18">
+      <c r="H9" s="13">
         <v>45659</v>
       </c>
-      <c r="I9" s="19">
+      <c r="I9" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -13439,10 +13761,10 @@
       <c r="G10" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H10" s="18">
+      <c r="H10" s="13">
         <v>45659</v>
       </c>
-      <c r="I10" s="19">
+      <c r="I10" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -13468,10 +13790,10 @@
       <c r="G11" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H11" s="18">
+      <c r="H11" s="13">
         <v>45659</v>
       </c>
-      <c r="I11" s="19">
+      <c r="I11" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -13497,10 +13819,10 @@
       <c r="G12" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H12" s="18">
+      <c r="H12" s="13">
         <v>45659</v>
       </c>
-      <c r="I12" s="19">
+      <c r="I12" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -13526,10 +13848,10 @@
       <c r="G13" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H13" s="18">
+      <c r="H13" s="13">
         <v>45659</v>
       </c>
-      <c r="I13" s="19">
+      <c r="I13" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -13555,10 +13877,10 @@
       <c r="G14" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H14" s="18">
+      <c r="H14" s="13">
         <v>45659</v>
       </c>
-      <c r="I14" s="19">
+      <c r="I14" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -13584,10 +13906,10 @@
       <c r="G15" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H15" s="18">
+      <c r="H15" s="13">
         <v>45659</v>
       </c>
-      <c r="I15" s="19">
+      <c r="I15" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -13613,10 +13935,10 @@
       <c r="G16" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H16" s="18">
+      <c r="H16" s="13">
         <v>45659</v>
       </c>
-      <c r="I16" s="19">
+      <c r="I16" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -13642,10 +13964,10 @@
       <c r="G17" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H17" s="18">
+      <c r="H17" s="13">
         <v>45659</v>
       </c>
-      <c r="I17" s="19">
+      <c r="I17" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -13671,10 +13993,10 @@
       <c r="G18" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H18" s="18">
+      <c r="H18" s="13">
         <v>45659</v>
       </c>
-      <c r="I18" s="19">
+      <c r="I18" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -13700,10 +14022,10 @@
       <c r="G19" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H19" s="18">
+      <c r="H19" s="13">
         <v>45659</v>
       </c>
-      <c r="I19" s="19">
+      <c r="I19" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -13729,10 +14051,10 @@
       <c r="G20" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H20" s="18">
+      <c r="H20" s="13">
         <v>45659</v>
       </c>
-      <c r="I20" s="19">
+      <c r="I20" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -13758,10 +14080,10 @@
       <c r="G21" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H21" s="18">
+      <c r="H21" s="13">
         <v>45659</v>
       </c>
-      <c r="I21" s="19">
+      <c r="I21" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -13787,10 +14109,10 @@
       <c r="G22" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H22" s="18">
+      <c r="H22" s="13">
         <v>45659</v>
       </c>
-      <c r="I22" s="19">
+      <c r="I22" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -13816,10 +14138,10 @@
       <c r="G23" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H23" s="18">
+      <c r="H23" s="13">
         <v>45659</v>
       </c>
-      <c r="I23" s="19">
+      <c r="I23" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -13845,10 +14167,10 @@
       <c r="G24" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H24" s="18">
+      <c r="H24" s="13">
         <v>45659</v>
       </c>
-      <c r="I24" s="19">
+      <c r="I24" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -13874,10 +14196,10 @@
       <c r="G25" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H25" s="18">
+      <c r="H25" s="13">
         <v>45659</v>
       </c>
-      <c r="I25" s="19">
+      <c r="I25" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -13903,10 +14225,10 @@
       <c r="G26" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H26" s="18">
+      <c r="H26" s="13">
         <v>45659</v>
       </c>
-      <c r="I26" s="19">
+      <c r="I26" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -13932,10 +14254,10 @@
       <c r="G27" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H27" s="18">
+      <c r="H27" s="13">
         <v>45659</v>
       </c>
-      <c r="I27" s="19">
+      <c r="I27" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -13961,10 +14283,10 @@
       <c r="G28" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H28" s="18">
+      <c r="H28" s="13">
         <v>45659</v>
       </c>
-      <c r="I28" s="19">
+      <c r="I28" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -13990,10 +14312,10 @@
       <c r="G29" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H29" s="18">
+      <c r="H29" s="13">
         <v>45659</v>
       </c>
-      <c r="I29" s="19">
+      <c r="I29" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -14019,10 +14341,10 @@
       <c r="G30" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H30" s="18">
+      <c r="H30" s="13">
         <v>45659</v>
       </c>
-      <c r="I30" s="19">
+      <c r="I30" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -14048,10 +14370,10 @@
       <c r="G31" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H31" s="18">
+      <c r="H31" s="13">
         <v>45659</v>
       </c>
-      <c r="I31" s="19">
+      <c r="I31" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -14077,10 +14399,10 @@
       <c r="G32" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H32" s="18">
+      <c r="H32" s="13">
         <v>45659</v>
       </c>
-      <c r="I32" s="19">
+      <c r="I32" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -14106,10 +14428,10 @@
       <c r="G33" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H33" s="18">
+      <c r="H33" s="13">
         <v>45659</v>
       </c>
-      <c r="I33" s="19">
+      <c r="I33" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -14135,10 +14457,10 @@
       <c r="G34" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H34" s="18">
+      <c r="H34" s="13">
         <v>45659</v>
       </c>
-      <c r="I34" s="19">
+      <c r="I34" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -14164,10 +14486,10 @@
       <c r="G35" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H35" s="18">
+      <c r="H35" s="13">
         <v>45659</v>
       </c>
-      <c r="I35" s="19">
+      <c r="I35" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -14193,10 +14515,10 @@
       <c r="G36" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H36" s="18">
+      <c r="H36" s="13">
         <v>45659</v>
       </c>
-      <c r="I36" s="19">
+      <c r="I36" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -14222,10 +14544,10 @@
       <c r="G37" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H37" s="18">
+      <c r="H37" s="13">
         <v>45659</v>
       </c>
-      <c r="I37" s="19">
+      <c r="I37" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -14251,10 +14573,10 @@
       <c r="G38" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H38" s="18">
+      <c r="H38" s="13">
         <v>45659</v>
       </c>
-      <c r="I38" s="19">
+      <c r="I38" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -14280,10 +14602,10 @@
       <c r="G39" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H39" s="18">
+      <c r="H39" s="13">
         <v>45659</v>
       </c>
-      <c r="I39" s="19">
+      <c r="I39" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -14309,10 +14631,10 @@
       <c r="G40" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H40" s="18">
+      <c r="H40" s="13">
         <v>45659</v>
       </c>
-      <c r="I40" s="19">
+      <c r="I40" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -14338,10 +14660,10 @@
       <c r="G41" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H41" s="18">
+      <c r="H41" s="13">
         <v>45659</v>
       </c>
-      <c r="I41" s="19">
+      <c r="I41" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -14367,10 +14689,10 @@
       <c r="G42" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H42" s="18">
+      <c r="H42" s="13">
         <v>45659</v>
       </c>
-      <c r="I42" s="19">
+      <c r="I42" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -14396,10 +14718,10 @@
       <c r="G43" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H43" s="18">
+      <c r="H43" s="13">
         <v>45659</v>
       </c>
-      <c r="I43" s="19">
+      <c r="I43" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -14425,10 +14747,10 @@
       <c r="G44" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H44" s="18">
+      <c r="H44" s="13">
         <v>45659</v>
       </c>
-      <c r="I44" s="19">
+      <c r="I44" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -14454,10 +14776,10 @@
       <c r="G45" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H45" s="18">
+      <c r="H45" s="13">
         <v>45659</v>
       </c>
-      <c r="I45" s="19">
+      <c r="I45" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -14483,10 +14805,10 @@
       <c r="G46" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H46" s="18">
+      <c r="H46" s="13">
         <v>45659</v>
       </c>
-      <c r="I46" s="19">
+      <c r="I46" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -14512,10 +14834,10 @@
       <c r="G47" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H47" s="18">
+      <c r="H47" s="13">
         <v>45659</v>
       </c>
-      <c r="I47" s="19">
+      <c r="I47" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -14541,10 +14863,10 @@
       <c r="G48" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H48" s="18">
+      <c r="H48" s="13">
         <v>45659</v>
       </c>
-      <c r="I48" s="19">
+      <c r="I48" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -14570,10 +14892,10 @@
       <c r="G49" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H49" s="18">
+      <c r="H49" s="13">
         <v>45659</v>
       </c>
-      <c r="I49" s="19">
+      <c r="I49" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -14599,10 +14921,10 @@
       <c r="G50" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H50" s="18">
+      <c r="H50" s="13">
         <v>45659</v>
       </c>
-      <c r="I50" s="19">
+      <c r="I50" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -14628,10 +14950,10 @@
       <c r="G51" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H51" s="18">
+      <c r="H51" s="13">
         <v>45659</v>
       </c>
-      <c r="I51" s="19">
+      <c r="I51" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -14657,10 +14979,10 @@
       <c r="G52" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H52" s="18">
+      <c r="H52" s="13">
         <v>45659</v>
       </c>
-      <c r="I52" s="19">
+      <c r="I52" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -14686,10 +15008,10 @@
       <c r="G53" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H53" s="18">
+      <c r="H53" s="13">
         <v>45659</v>
       </c>
-      <c r="I53" s="19">
+      <c r="I53" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -14715,10 +15037,10 @@
       <c r="G54" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H54" s="18">
+      <c r="H54" s="13">
         <v>45659</v>
       </c>
-      <c r="I54" s="19">
+      <c r="I54" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -14744,10 +15066,10 @@
       <c r="G55" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H55" s="18">
+      <c r="H55" s="13">
         <v>45659</v>
       </c>
-      <c r="I55" s="19">
+      <c r="I55" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -14773,10 +15095,10 @@
       <c r="G56" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H56" s="18">
+      <c r="H56" s="13">
         <v>45659</v>
       </c>
-      <c r="I56" s="19">
+      <c r="I56" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -14802,10 +15124,10 @@
       <c r="G57" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H57" s="18">
+      <c r="H57" s="13">
         <v>45659</v>
       </c>
-      <c r="I57" s="19">
+      <c r="I57" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -14831,10 +15153,10 @@
       <c r="G58" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H58" s="18">
+      <c r="H58" s="13">
         <v>45659</v>
       </c>
-      <c r="I58" s="19">
+      <c r="I58" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -14860,10 +15182,10 @@
       <c r="G59" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H59" s="18">
+      <c r="H59" s="13">
         <v>45659</v>
       </c>
-      <c r="I59" s="19">
+      <c r="I59" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -14889,10 +15211,10 @@
       <c r="G60" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H60" s="18">
+      <c r="H60" s="13">
         <v>45659</v>
       </c>
-      <c r="I60" s="19">
+      <c r="I60" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -14918,10 +15240,10 @@
       <c r="G61" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H61" s="18">
+      <c r="H61" s="13">
         <v>45659</v>
       </c>
-      <c r="I61" s="19">
+      <c r="I61" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -14947,10 +15269,10 @@
       <c r="G62" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H62" s="18">
+      <c r="H62" s="13">
         <v>45659</v>
       </c>
-      <c r="I62" s="19">
+      <c r="I62" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -14976,10 +15298,10 @@
       <c r="G63" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H63" s="18">
+      <c r="H63" s="13">
         <v>45659</v>
       </c>
-      <c r="I63" s="19">
+      <c r="I63" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -15005,10 +15327,10 @@
       <c r="G64" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H64" s="18">
+      <c r="H64" s="13">
         <v>45659</v>
       </c>
-      <c r="I64" s="19">
+      <c r="I64" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -15034,10 +15356,10 @@
       <c r="G65" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H65" s="18">
+      <c r="H65" s="13">
         <v>45659</v>
       </c>
-      <c r="I65" s="19">
+      <c r="I65" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -15063,10 +15385,10 @@
       <c r="G66" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H66" s="18">
+      <c r="H66" s="13">
         <v>45659</v>
       </c>
-      <c r="I66" s="19">
+      <c r="I66" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -15092,10 +15414,10 @@
       <c r="G67" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H67" s="18">
+      <c r="H67" s="13">
         <v>45659</v>
       </c>
-      <c r="I67" s="19">
+      <c r="I67" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -15121,10 +15443,10 @@
       <c r="G68" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H68" s="18">
+      <c r="H68" s="13">
         <v>45659</v>
       </c>
-      <c r="I68" s="19">
+      <c r="I68" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -15150,10 +15472,10 @@
       <c r="G69" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H69" s="18">
+      <c r="H69" s="13">
         <v>45659</v>
       </c>
-      <c r="I69" s="19">
+      <c r="I69" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -15179,10 +15501,10 @@
       <c r="G70" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H70" s="18">
+      <c r="H70" s="13">
         <v>45659</v>
       </c>
-      <c r="I70" s="19">
+      <c r="I70" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -15208,10 +15530,10 @@
       <c r="G71" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H71" s="18">
+      <c r="H71" s="13">
         <v>45659</v>
       </c>
-      <c r="I71" s="19">
+      <c r="I71" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -15237,10 +15559,10 @@
       <c r="G72" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H72" s="18">
+      <c r="H72" s="13">
         <v>45659</v>
       </c>
-      <c r="I72" s="19">
+      <c r="I72" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -15266,10 +15588,10 @@
       <c r="G73" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H73" s="18">
+      <c r="H73" s="13">
         <v>45659</v>
       </c>
-      <c r="I73" s="19">
+      <c r="I73" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -15295,10 +15617,10 @@
       <c r="G74" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H74" s="18">
+      <c r="H74" s="13">
         <v>45659</v>
       </c>
-      <c r="I74" s="19">
+      <c r="I74" s="6">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -15313,10 +15635,10 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D2">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D74">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15326,8 +15648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5113C119-7BB4-4304-A88E-D0533852E833}">
   <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:G74"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15409,11 +15731,11 @@
       <c r="G3" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H3" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I3" s="19" t="s">
-        <v>1007</v>
+      <c r="H3" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I3" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -15438,11 +15760,11 @@
       <c r="G4" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H4" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I4" s="19" t="s">
-        <v>1007</v>
+      <c r="H4" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -15467,11 +15789,11 @@
       <c r="G5" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H5" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I5" s="19" t="s">
-        <v>1007</v>
+      <c r="H5" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -15496,11 +15818,11 @@
       <c r="G6" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H6" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I6" s="19" t="s">
-        <v>1007</v>
+      <c r="H6" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I6" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -15525,11 +15847,11 @@
       <c r="G7" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H7" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I7" s="19" t="s">
-        <v>1007</v>
+      <c r="H7" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I7" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -15554,11 +15876,11 @@
       <c r="G8" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H8" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I8" s="19" t="s">
-        <v>1007</v>
+      <c r="H8" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I8" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -15583,11 +15905,11 @@
       <c r="G9" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H9" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I9" s="19" t="s">
-        <v>1007</v>
+      <c r="H9" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I9" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -15612,11 +15934,11 @@
       <c r="G10" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H10" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I10" s="19" t="s">
-        <v>1007</v>
+      <c r="H10" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I10" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -15641,11 +15963,11 @@
       <c r="G11" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H11" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I11" s="19" t="s">
-        <v>1007</v>
+      <c r="H11" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I11" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -15670,11 +15992,11 @@
       <c r="G12" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H12" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I12" s="19" t="s">
-        <v>1007</v>
+      <c r="H12" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -15699,11 +16021,11 @@
       <c r="G13" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H13" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I13" s="19" t="s">
-        <v>1007</v>
+      <c r="H13" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I13" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -15728,11 +16050,11 @@
       <c r="G14" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H14" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I14" s="19" t="s">
-        <v>1007</v>
+      <c r="H14" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I14" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -15757,11 +16079,11 @@
       <c r="G15" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H15" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I15" s="19" t="s">
-        <v>1007</v>
+      <c r="H15" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I15" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -15786,11 +16108,11 @@
       <c r="G16" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H16" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I16" s="19" t="s">
-        <v>1007</v>
+      <c r="H16" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I16" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -15815,11 +16137,11 @@
       <c r="G17" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H17" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I17" s="19" t="s">
-        <v>1007</v>
+      <c r="H17" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I17" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -15844,11 +16166,11 @@
       <c r="G18" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H18" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I18" s="19" t="s">
-        <v>1007</v>
+      <c r="H18" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I18" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -15873,11 +16195,11 @@
       <c r="G19" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H19" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I19" s="19" t="s">
-        <v>1007</v>
+      <c r="H19" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I19" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -15902,11 +16224,11 @@
       <c r="G20" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H20" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I20" s="19" t="s">
-        <v>1007</v>
+      <c r="H20" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I20" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -15931,11 +16253,11 @@
       <c r="G21" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H21" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I21" s="19" t="s">
-        <v>1007</v>
+      <c r="H21" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I21" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -15960,11 +16282,11 @@
       <c r="G22" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H22" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I22" s="19" t="s">
-        <v>1007</v>
+      <c r="H22" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I22" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -15989,11 +16311,11 @@
       <c r="G23" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H23" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I23" s="19" t="s">
-        <v>1007</v>
+      <c r="H23" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I23" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -16018,11 +16340,11 @@
       <c r="G24" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H24" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I24" s="19" t="s">
-        <v>1007</v>
+      <c r="H24" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I24" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -16047,11 +16369,11 @@
       <c r="G25" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H25" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I25" s="19" t="s">
-        <v>1007</v>
+      <c r="H25" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I25" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -16076,11 +16398,11 @@
       <c r="G26" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H26" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I26" s="19" t="s">
-        <v>1007</v>
+      <c r="H26" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I26" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -16105,11 +16427,11 @@
       <c r="G27" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H27" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I27" s="19" t="s">
-        <v>1007</v>
+      <c r="H27" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I27" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -16134,11 +16456,11 @@
       <c r="G28" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H28" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I28" s="19" t="s">
-        <v>1007</v>
+      <c r="H28" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I28" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -16163,11 +16485,11 @@
       <c r="G29" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H29" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I29" s="19" t="s">
-        <v>1007</v>
+      <c r="H29" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I29" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -16192,11 +16514,11 @@
       <c r="G30" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H30" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I30" s="19" t="s">
-        <v>1007</v>
+      <c r="H30" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I30" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -16221,11 +16543,11 @@
       <c r="G31" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H31" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I31" s="19" t="s">
-        <v>1007</v>
+      <c r="H31" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I31" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -16250,11 +16572,11 @@
       <c r="G32" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H32" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I32" s="19" t="s">
-        <v>1007</v>
+      <c r="H32" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I32" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -16279,11 +16601,11 @@
       <c r="G33" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H33" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I33" s="19" t="s">
-        <v>1007</v>
+      <c r="H33" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I33" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -16308,11 +16630,11 @@
       <c r="G34" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H34" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I34" s="19" t="s">
-        <v>1007</v>
+      <c r="H34" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I34" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -16337,11 +16659,11 @@
       <c r="G35" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H35" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I35" s="19" t="s">
-        <v>1007</v>
+      <c r="H35" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I35" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -16366,11 +16688,11 @@
       <c r="G36" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H36" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I36" s="19" t="s">
-        <v>1007</v>
+      <c r="H36" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I36" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -16395,11 +16717,11 @@
       <c r="G37" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H37" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I37" s="19" t="s">
-        <v>1007</v>
+      <c r="H37" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I37" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -16424,11 +16746,11 @@
       <c r="G38" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H38" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I38" s="19" t="s">
-        <v>1007</v>
+      <c r="H38" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I38" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -16453,11 +16775,11 @@
       <c r="G39" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H39" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I39" s="19" t="s">
-        <v>1007</v>
+      <c r="H39" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I39" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -16482,11 +16804,11 @@
       <c r="G40" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H40" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I40" s="19" t="s">
-        <v>1007</v>
+      <c r="H40" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I40" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -16511,11 +16833,11 @@
       <c r="G41" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H41" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I41" s="19" t="s">
-        <v>1007</v>
+      <c r="H41" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I41" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -16540,11 +16862,11 @@
       <c r="G42" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H42" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I42" s="19" t="s">
-        <v>1007</v>
+      <c r="H42" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I42" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -16569,11 +16891,11 @@
       <c r="G43" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H43" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I43" s="19" t="s">
-        <v>1007</v>
+      <c r="H43" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I43" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -16598,11 +16920,11 @@
       <c r="G44" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H44" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I44" s="19" t="s">
-        <v>1007</v>
+      <c r="H44" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I44" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -16627,11 +16949,11 @@
       <c r="G45" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H45" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I45" s="19" t="s">
-        <v>1007</v>
+      <c r="H45" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I45" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -16656,11 +16978,11 @@
       <c r="G46" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H46" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I46" s="19" t="s">
-        <v>1007</v>
+      <c r="H46" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I46" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -16685,11 +17007,11 @@
       <c r="G47" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H47" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I47" s="19" t="s">
-        <v>1007</v>
+      <c r="H47" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I47" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -16714,11 +17036,11 @@
       <c r="G48" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H48" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I48" s="19" t="s">
-        <v>1007</v>
+      <c r="H48" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I48" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -16743,11 +17065,11 @@
       <c r="G49" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H49" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I49" s="19" t="s">
-        <v>1007</v>
+      <c r="H49" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I49" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -16772,11 +17094,11 @@
       <c r="G50" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H50" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I50" s="19" t="s">
-        <v>1007</v>
+      <c r="H50" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I50" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -16801,11 +17123,11 @@
       <c r="G51" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H51" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I51" s="19" t="s">
-        <v>1007</v>
+      <c r="H51" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I51" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -16830,11 +17152,11 @@
       <c r="G52" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H52" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I52" s="19" t="s">
-        <v>1007</v>
+      <c r="H52" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I52" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -16859,11 +17181,11 @@
       <c r="G53" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H53" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I53" s="19" t="s">
-        <v>1007</v>
+      <c r="H53" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I53" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -16888,11 +17210,11 @@
       <c r="G54" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H54" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I54" s="19" t="s">
-        <v>1007</v>
+      <c r="H54" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I54" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -16917,11 +17239,11 @@
       <c r="G55" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H55" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I55" s="19" t="s">
-        <v>1007</v>
+      <c r="H55" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I55" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -16946,11 +17268,11 @@
       <c r="G56" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H56" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I56" s="19" t="s">
-        <v>1007</v>
+      <c r="H56" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I56" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -16975,11 +17297,11 @@
       <c r="G57" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H57" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I57" s="19" t="s">
-        <v>1007</v>
+      <c r="H57" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I57" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -17004,11 +17326,11 @@
       <c r="G58" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H58" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I58" s="19" t="s">
-        <v>1007</v>
+      <c r="H58" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I58" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -17033,11 +17355,11 @@
       <c r="G59" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H59" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I59" s="19" t="s">
-        <v>1007</v>
+      <c r="H59" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I59" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -17062,11 +17384,11 @@
       <c r="G60" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H60" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I60" s="19" t="s">
-        <v>1007</v>
+      <c r="H60" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I60" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -17091,11 +17413,11 @@
       <c r="G61" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H61" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I61" s="19" t="s">
-        <v>1007</v>
+      <c r="H61" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I61" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -17120,11 +17442,11 @@
       <c r="G62" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H62" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I62" s="19" t="s">
-        <v>1007</v>
+      <c r="H62" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I62" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -17149,11 +17471,11 @@
       <c r="G63" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H63" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I63" s="19" t="s">
-        <v>1007</v>
+      <c r="H63" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I63" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -17178,11 +17500,11 @@
       <c r="G64" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H64" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I64" s="19" t="s">
-        <v>1007</v>
+      <c r="H64" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I64" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -17207,11 +17529,11 @@
       <c r="G65" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H65" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I65" s="19" t="s">
-        <v>1007</v>
+      <c r="H65" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I65" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -17236,11 +17558,11 @@
       <c r="G66" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H66" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I66" s="19" t="s">
-        <v>1007</v>
+      <c r="H66" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I66" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -17265,11 +17587,11 @@
       <c r="G67" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H67" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I67" s="19" t="s">
-        <v>1007</v>
+      <c r="H67" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I67" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -17294,11 +17616,11 @@
       <c r="G68" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H68" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I68" s="19" t="s">
-        <v>1007</v>
+      <c r="H68" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I68" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -17323,11 +17645,11 @@
       <c r="G69" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H69" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I69" s="19" t="s">
-        <v>1007</v>
+      <c r="H69" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I69" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -17352,11 +17674,11 @@
       <c r="G70" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H70" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I70" s="19" t="s">
-        <v>1007</v>
+      <c r="H70" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I70" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -17381,11 +17703,11 @@
       <c r="G71" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H71" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I71" s="19" t="s">
-        <v>1007</v>
+      <c r="H71" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I71" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -17410,11 +17732,11 @@
       <c r="G72" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H72" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I72" s="19" t="s">
-        <v>1007</v>
+      <c r="H72" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I72" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -17439,11 +17761,11 @@
       <c r="G73" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H73" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I73" s="19" t="s">
-        <v>1007</v>
+      <c r="H73" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I73" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -17468,11 +17790,11 @@
       <c r="G74" s="6">
         <v>0.46875</v>
       </c>
-      <c r="H74" s="18" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I74" s="19" t="s">
-        <v>1007</v>
+      <c r="H74" s="13">
+        <v>45660</v>
+      </c>
+      <c r="I74" s="6">
+        <v>0.39583333333333331</v>
       </c>
     </row>
   </sheetData>
@@ -17486,10 +17808,2197 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D2">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D74">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90C24B94-54EF-4112-9AA1-A1C421C8AF9A}">
+  <dimension ref="A1:I74"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="74" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.21875" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="17"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>1234</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>1235</v>
+      </c>
+      <c r="E3" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F3" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G3" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>1234</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>1236</v>
+      </c>
+      <c r="E4" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F4" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G4" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>1234</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>1237</v>
+      </c>
+      <c r="E5" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F5" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G5" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>1234</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>1238</v>
+      </c>
+      <c r="E6" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F6" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G6" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>1234</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>1239</v>
+      </c>
+      <c r="E7" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F7" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G7" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>1234</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>1240</v>
+      </c>
+      <c r="E8" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F8" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G8" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>1234</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>1241</v>
+      </c>
+      <c r="E9" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F9" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G9" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>1234</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>1242</v>
+      </c>
+      <c r="E10" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F10" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G10" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>1234</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>1243</v>
+      </c>
+      <c r="E11" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F11" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G11" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>1234</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>1244</v>
+      </c>
+      <c r="E12" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F12" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G12" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>1234</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>1245</v>
+      </c>
+      <c r="E13" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F13" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G13" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>1234</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>1246</v>
+      </c>
+      <c r="E14" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F14" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G14" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>1234</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>1247</v>
+      </c>
+      <c r="E15" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F15" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G15" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>1234</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>1248</v>
+      </c>
+      <c r="E16" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F16" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G16" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>1234</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>1249</v>
+      </c>
+      <c r="E17" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F17" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G17" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>1234</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>1250</v>
+      </c>
+      <c r="E18" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F18" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G18" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>17</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>1234</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>1251</v>
+      </c>
+      <c r="E19" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F19" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G19" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>18</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>1234</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>1252</v>
+      </c>
+      <c r="E20" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F20" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G20" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>19</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>1253</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>1254</v>
+      </c>
+      <c r="E21" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F21" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G21" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>20</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>1253</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>1255</v>
+      </c>
+      <c r="E22" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F22" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G22" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>21</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>1253</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>1256</v>
+      </c>
+      <c r="E23" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F23" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G23" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>22</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>1253</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>1257</v>
+      </c>
+      <c r="E24" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F24" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G24" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I24" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>23</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>1253</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>1258</v>
+      </c>
+      <c r="E25" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F25" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G25" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I25" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>24</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>1253</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>1259</v>
+      </c>
+      <c r="E26" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F26" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G26" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I26" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>25</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>1253</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>1260</v>
+      </c>
+      <c r="E27" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F27" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G27" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I27" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>26</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>1253</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>1261</v>
+      </c>
+      <c r="E28" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F28" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G28" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I28" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>27</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>1253</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>1262</v>
+      </c>
+      <c r="E29" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F29" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G29" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H29" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I29" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>28</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>1253</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>1263</v>
+      </c>
+      <c r="E30" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F30" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G30" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I30" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <v>29</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>1253</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>1264</v>
+      </c>
+      <c r="E31" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F31" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G31" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H31" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I31" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <v>30</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>1253</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>1265</v>
+      </c>
+      <c r="E32" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F32" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G32" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I32" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
+        <v>31</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>1253</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>1266</v>
+      </c>
+      <c r="E33" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F33" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G33" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H33" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I33" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
+        <v>32</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>1253</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>1267</v>
+      </c>
+      <c r="E34" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F34" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G34" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H34" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I34" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
+        <v>33</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>1253</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>1268</v>
+      </c>
+      <c r="E35" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F35" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G35" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I35" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
+        <v>34</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>1253</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>1269</v>
+      </c>
+      <c r="E36" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F36" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G36" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H36" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I36" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
+        <v>35</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>1253</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>1270</v>
+      </c>
+      <c r="E37" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F37" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G37" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H37" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I37" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="2">
+        <v>36</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>1253</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>1271</v>
+      </c>
+      <c r="E38" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F38" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G38" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H38" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I38" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
+        <v>37</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>1272</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>1273</v>
+      </c>
+      <c r="E39" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F39" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G39" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H39" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I39" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="2">
+        <v>38</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>1272</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>1274</v>
+      </c>
+      <c r="E40" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F40" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G40" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H40" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I40" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" s="2">
+        <v>39</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>1272</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>1275</v>
+      </c>
+      <c r="E41" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F41" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G41" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H41" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I41" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" s="2">
+        <v>40</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>1272</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E42" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F42" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G42" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H42" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I42" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" s="2">
+        <v>41</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>1272</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>1277</v>
+      </c>
+      <c r="E43" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F43" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G43" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H43" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I43" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" s="2">
+        <v>42</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>1272</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>1278</v>
+      </c>
+      <c r="E44" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F44" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G44" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H44" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I44" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" s="2">
+        <v>43</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>1272</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>1279</v>
+      </c>
+      <c r="E45" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F45" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G45" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H45" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I45" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" s="2">
+        <v>44</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C46" s="18" t="s">
+        <v>1272</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>1280</v>
+      </c>
+      <c r="E46" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F46" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G46" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H46" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I46" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" s="2">
+        <v>45</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C47" s="18" t="s">
+        <v>1272</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>1281</v>
+      </c>
+      <c r="E47" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F47" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G47" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H47" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I47" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" s="2">
+        <v>46</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C48" s="18" t="s">
+        <v>1272</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>1282</v>
+      </c>
+      <c r="E48" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F48" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G48" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H48" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I48" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" s="2">
+        <v>47</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C49" s="18" t="s">
+        <v>1272</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>1283</v>
+      </c>
+      <c r="E49" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F49" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G49" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H49" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I49" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" s="2">
+        <v>48</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C50" s="18" t="s">
+        <v>1272</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>1284</v>
+      </c>
+      <c r="E50" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F50" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G50" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H50" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I50" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" s="2">
+        <v>49</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C51" s="18" t="s">
+        <v>1272</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="E51" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F51" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G51" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H51" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I51" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" s="2">
+        <v>50</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C52" s="18" t="s">
+        <v>1272</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>1286</v>
+      </c>
+      <c r="E52" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F52" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G52" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H52" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I52" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" s="2">
+        <v>51</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C53" s="18" t="s">
+        <v>1272</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>1287</v>
+      </c>
+      <c r="E53" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F53" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G53" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H53" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I53" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54" s="2">
+        <v>52</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C54" s="18" t="s">
+        <v>1272</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>1288</v>
+      </c>
+      <c r="E54" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F54" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G54" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H54" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I54" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" s="2">
+        <v>53</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C55" s="18" t="s">
+        <v>1272</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>1289</v>
+      </c>
+      <c r="E55" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F55" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G55" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H55" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I55" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" s="2">
+        <v>54</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C56" s="18" t="s">
+        <v>1272</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>1290</v>
+      </c>
+      <c r="E56" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F56" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G56" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H56" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I56" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57" s="2">
+        <v>55</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C57" s="18" t="s">
+        <v>1291</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="E57" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F57" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G57" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H57" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I57" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58" s="2">
+        <v>56</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C58" s="18" t="s">
+        <v>1291</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="E58" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F58" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G58" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H58" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I58" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59" s="2">
+        <v>57</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C59" s="18" t="s">
+        <v>1291</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>1294</v>
+      </c>
+      <c r="E59" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F59" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G59" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H59" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I59" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" s="2">
+        <v>58</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C60" s="18" t="s">
+        <v>1291</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>1295</v>
+      </c>
+      <c r="E60" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F60" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G60" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H60" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I60" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A61" s="2">
+        <v>59</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C61" s="18" t="s">
+        <v>1291</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>1296</v>
+      </c>
+      <c r="E61" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F61" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G61" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H61" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I61" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62" s="2">
+        <v>60</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C62" s="18" t="s">
+        <v>1291</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>1297</v>
+      </c>
+      <c r="E62" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F62" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G62" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H62" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I62" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63" s="2">
+        <v>61</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C63" s="18" t="s">
+        <v>1291</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="E63" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F63" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G63" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H63" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I63" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64" s="2">
+        <v>62</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C64" s="18" t="s">
+        <v>1291</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>1299</v>
+      </c>
+      <c r="E64" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F64" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G64" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H64" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I64" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A65" s="2">
+        <v>63</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C65" s="18" t="s">
+        <v>1291</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>1300</v>
+      </c>
+      <c r="E65" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F65" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G65" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H65" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I65" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A66" s="2">
+        <v>64</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C66" s="18" t="s">
+        <v>1291</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>1301</v>
+      </c>
+      <c r="E66" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F66" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G66" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H66" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I66" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A67" s="2">
+        <v>65</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C67" s="18" t="s">
+        <v>1291</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>1302</v>
+      </c>
+      <c r="E67" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F67" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G67" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H67" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I67" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A68" s="2">
+        <v>66</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C68" s="18" t="s">
+        <v>1291</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>1303</v>
+      </c>
+      <c r="E68" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F68" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G68" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H68" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I68" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A69" s="2">
+        <v>67</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C69" s="18" t="s">
+        <v>1291</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>1304</v>
+      </c>
+      <c r="E69" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F69" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G69" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H69" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I69" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A70" s="2">
+        <v>68</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C70" s="18" t="s">
+        <v>1291</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>1305</v>
+      </c>
+      <c r="E70" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F70" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G70" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H70" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I70" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A71" s="2">
+        <v>69</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C71" s="18" t="s">
+        <v>1291</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>1306</v>
+      </c>
+      <c r="E71" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F71" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G71" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H71" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I71" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A72" s="2">
+        <v>70</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C72" s="18" t="s">
+        <v>1291</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>1307</v>
+      </c>
+      <c r="E72" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F72" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G72" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H72" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I72" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A73" s="2">
+        <v>71</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C73" s="18" t="s">
+        <v>1291</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>1308</v>
+      </c>
+      <c r="E73" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F73" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G73" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H73" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I73" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A74" s="2">
+        <v>72</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C74" s="18" t="s">
+        <v>1291</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>1309</v>
+      </c>
+      <c r="E74" s="18">
+        <v>801983371</v>
+      </c>
+      <c r="F74" s="19">
+        <v>45660</v>
+      </c>
+      <c r="G74" s="20">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="H74" s="13" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I74" s="13" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D1:D2">
+    <cfRule type="duplicateValues" dxfId="8" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D20">
+    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D56">
+    <cfRule type="duplicateValues" dxfId="5" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D74">
+    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="9"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D21:D38">
+    <cfRule type="duplicateValues" dxfId="2" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D39:D56">
+    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="6"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -21747,7 +24256,7 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="duplicateValues" dxfId="16" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -21760,7 +24269,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A836090B-1D84-488F-9E82-01BA25B98056}">
   <dimension ref="A1:I146"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="H1" sqref="H1:I1"/>
     </sheetView>
   </sheetViews>
@@ -26008,7 +28517,7 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D74">
-    <cfRule type="duplicateValues" dxfId="15" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -26021,7 +28530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78193475-AAD8-4321-A269-9105EF47F6A1}">
   <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView topLeftCell="A66" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
@@ -28184,7 +30693,7 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D74">
-    <cfRule type="duplicateValues" dxfId="14" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -28194,8 +30703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E89FE45D-4AA5-4CA0-BB33-3B7270B8095F}">
   <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E74"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30354,7 +32863,7 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D74">
-    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -30364,8 +32873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{478E4E42-F398-4C65-BF3C-2DE2ABC0E541}">
   <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="H76" sqref="H76"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32524,7 +35033,7 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D74">
-    <cfRule type="duplicateValues" dxfId="12" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -32534,7 +35043,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F70B6AA-5825-49A8-A25A-422DAEE45532}">
   <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView topLeftCell="A66" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J80" sqref="J80"/>
     </sheetView>
   </sheetViews>
@@ -34694,7 +37203,7 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D74">
-    <cfRule type="duplicateValues" dxfId="11" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -36863,7 +39372,7 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D74">
-    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -39033,7 +41542,7 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D74">
-    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>